<commit_message>
bug fix and results update
</commit_message>
<xml_diff>
--- a/results/result_summary_epsilon_support.xlsx
+++ b/results/result_summary_epsilon_support.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Robert\Documents\_Work\Research\00_Workshop\data_valuation\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39DFB1ED-7930-4614-9A83-605F65D642A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EED0A275-21CC-40B5-A05B-78C03940762D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{FFE2B131-66A4-4E63-8C13-A75AF38B9E2B}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" activeTab="1" xr2:uid="{FFE2B131-66A4-4E63-8C13-A75AF38B9E2B}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="2" r:id="rId1"/>
@@ -477,7 +477,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{056EC552-3B33-4C7A-BFE0-F85E370CBE75}">
   <dimension ref="B2:C11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
@@ -570,8 +570,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BB6718F-3B8A-4B8D-842A-7EE6474384A0}">
   <dimension ref="B1:T66"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M9" sqref="M9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="U11" sqref="U11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -660,10 +660,10 @@
         <v>1</v>
       </c>
       <c r="D3" s="2">
-        <v>1923.0369508579699</v>
+        <v>0</v>
       </c>
       <c r="E3" s="2">
-        <v>2029.5577647417799</v>
+        <v>0</v>
       </c>
       <c r="G3">
         <v>1</v>
@@ -672,10 +672,10 @@
         <v>1</v>
       </c>
       <c r="I3" s="2">
-        <v>1283.8383224409899</v>
+        <v>0</v>
       </c>
       <c r="J3" s="2">
-        <v>1913.30625892486</v>
+        <v>0</v>
       </c>
       <c r="L3">
         <v>1</v>
@@ -684,10 +684,10 @@
         <v>1</v>
       </c>
       <c r="N3" s="2">
-        <v>2265.3053320951299</v>
+        <v>0</v>
       </c>
       <c r="O3" s="2">
-        <v>2265.3053320951299</v>
+        <v>0</v>
       </c>
       <c r="Q3">
         <v>1</v>
@@ -696,24 +696,24 @@
         <v>1</v>
       </c>
       <c r="S3" s="2">
-        <v>866.06943582979295</v>
+        <v>0</v>
       </c>
       <c r="T3" s="2">
-        <v>2046.1628228033101</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="2:20" x14ac:dyDescent="0.55000000000000004">
       <c r="B4">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="C4">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="D4" s="2">
-        <v>1864.96030533156</v>
+        <v>0</v>
       </c>
       <c r="E4" s="2">
-        <v>1988.14522133331</v>
+        <v>0</v>
       </c>
       <c r="G4">
         <v>0.5</v>
@@ -722,10 +722,10 @@
         <v>1</v>
       </c>
       <c r="I4" s="2">
-        <v>745.43606362372702</v>
+        <v>0</v>
       </c>
       <c r="J4" s="2">
-        <v>2130.97169776899</v>
+        <v>0</v>
       </c>
       <c r="L4">
         <v>0.5</v>
@@ -734,10 +734,10 @@
         <v>1</v>
       </c>
       <c r="N4" s="2">
-        <v>1995.1041474026499</v>
+        <v>0</v>
       </c>
       <c r="O4" s="2">
-        <v>2040.0517637320399</v>
+        <v>0</v>
       </c>
       <c r="Q4">
         <v>0.5</v>
@@ -746,24 +746,24 @@
         <v>1</v>
       </c>
       <c r="S4" s="2">
-        <v>931.11400958941795</v>
+        <v>0</v>
       </c>
       <c r="T4" s="2">
-        <v>1929.92316188014</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="2:20" x14ac:dyDescent="0.55000000000000004">
       <c r="B5">
-        <v>1</v>
+        <v>0.2</v>
       </c>
       <c r="C5">
-        <v>0.2</v>
+        <v>1</v>
       </c>
       <c r="D5" s="2">
-        <v>2038.13440695023</v>
+        <v>1774.7211885793499</v>
       </c>
       <c r="E5" s="2">
-        <v>2057.0361639522098</v>
+        <v>0</v>
       </c>
       <c r="G5">
         <v>0.2</v>
@@ -772,10 +772,10 @@
         <v>1</v>
       </c>
       <c r="I5" s="2">
-        <v>1161.10563706677</v>
+        <v>0</v>
       </c>
       <c r="J5" s="2">
-        <v>1911.12637178672</v>
+        <v>0</v>
       </c>
       <c r="L5">
         <v>0.2</v>
@@ -784,10 +784,10 @@
         <v>1</v>
       </c>
       <c r="N5" s="2">
-        <v>2267.42847834025</v>
+        <v>1855.95921197143</v>
       </c>
       <c r="O5" s="2">
-        <v>2531.3844269403398</v>
+        <v>0</v>
       </c>
       <c r="Q5">
         <v>0.2</v>
@@ -796,24 +796,24 @@
         <v>1</v>
       </c>
       <c r="S5" s="2">
-        <v>762.03577450426599</v>
+        <v>1025.9709953481699</v>
       </c>
       <c r="T5" s="2">
-        <v>1766.2122550423901</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="2:20" x14ac:dyDescent="0.55000000000000004">
       <c r="B6">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="C6">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="D6" s="2">
-        <v>2168.9557310908299</v>
+        <v>1821.5228289618899</v>
       </c>
       <c r="E6" s="2">
-        <v>2168.9557310908299</v>
+        <v>0</v>
       </c>
       <c r="G6">
         <v>0.1</v>
@@ -822,10 +822,10 @@
         <v>1</v>
       </c>
       <c r="I6" s="2">
-        <v>664.70563474880896</v>
+        <v>862.84691356399605</v>
       </c>
       <c r="J6" s="2">
-        <v>1716.8325746691701</v>
+        <v>0</v>
       </c>
       <c r="L6">
         <v>0.1</v>
@@ -834,10 +834,10 @@
         <v>1</v>
       </c>
       <c r="N6" s="2">
-        <v>2101.8015119045799</v>
+        <v>1818.4728810709901</v>
       </c>
       <c r="O6" s="2">
-        <v>2126.7110524754598</v>
+        <v>0</v>
       </c>
       <c r="Q6">
         <v>0.1</v>
@@ -846,24 +846,24 @@
         <v>1</v>
       </c>
       <c r="S6" s="2">
-        <v>629.27436066034795</v>
+        <v>1921.5473837582599</v>
       </c>
       <c r="T6" s="2">
-        <v>1632.2629284712</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="2:20" x14ac:dyDescent="0.55000000000000004">
       <c r="B7">
-        <v>1</v>
+        <v>0.05</v>
       </c>
       <c r="C7">
-        <v>0.05</v>
+        <v>1</v>
       </c>
       <c r="D7" s="2">
-        <v>2261.2659604166702</v>
+        <v>1971.8544722638401</v>
       </c>
       <c r="E7" s="2">
-        <v>2365.05758464878</v>
+        <v>0</v>
       </c>
       <c r="G7">
         <v>0.05</v>
@@ -872,10 +872,10 @@
         <v>1</v>
       </c>
       <c r="I7" s="2">
-        <v>984.95288290406302</v>
+        <v>1564.99392789282</v>
       </c>
       <c r="J7" s="2">
-        <v>1931.8216806395501</v>
+        <v>0</v>
       </c>
       <c r="L7">
         <v>0.05</v>
@@ -884,10 +884,10 @@
         <v>1</v>
       </c>
       <c r="N7" s="2">
-        <v>2292.66594395537</v>
+        <v>1755.1086326319601</v>
       </c>
       <c r="O7" s="2">
-        <v>2337.3301534723801</v>
+        <v>0</v>
       </c>
       <c r="Q7">
         <v>0.05</v>
@@ -896,24 +896,24 @@
         <v>1</v>
       </c>
       <c r="S7" s="2">
-        <v>1200.8751683830501</v>
+        <v>2064.8039404741498</v>
       </c>
       <c r="T7" s="2">
-        <v>2077.7521272101098</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="2:20" x14ac:dyDescent="0.55000000000000004">
       <c r="B8">
-        <v>1</v>
+        <v>0.01</v>
       </c>
       <c r="C8">
-        <v>0.01</v>
+        <v>1</v>
       </c>
       <c r="D8" s="2">
-        <v>2132.4941486093098</v>
+        <v>1807.1907572103</v>
       </c>
       <c r="E8" s="2">
-        <v>2132.4941486093098</v>
+        <v>0</v>
       </c>
       <c r="G8">
         <v>0.01</v>
@@ -922,10 +922,10 @@
         <v>1</v>
       </c>
       <c r="I8" s="2">
-        <v>887.21452860710997</v>
+        <v>1453.29138596096</v>
       </c>
       <c r="J8" s="2">
-        <v>1900.8851546026999</v>
+        <v>0</v>
       </c>
       <c r="L8">
         <v>0.01</v>
@@ -934,10 +934,10 @@
         <v>1</v>
       </c>
       <c r="N8" s="2">
-        <v>2019.9303631704699</v>
+        <v>2078.8307401534998</v>
       </c>
       <c r="O8" s="2">
-        <v>2035.81941741531</v>
+        <v>0</v>
       </c>
       <c r="Q8">
         <v>0.01</v>
@@ -946,24 +946,24 @@
         <v>1</v>
       </c>
       <c r="S8" s="2">
-        <v>824.19213174521803</v>
+        <v>2008.30155007959</v>
       </c>
       <c r="T8" s="2">
-        <v>1739.87861397753</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="2:20" x14ac:dyDescent="0.55000000000000004">
       <c r="B9">
-        <v>1</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="C9">
-        <v>5.0000000000000001E-3</v>
+        <v>1</v>
       </c>
       <c r="D9" s="2">
-        <v>2174.606135902</v>
+        <v>2261.2066057606698</v>
       </c>
       <c r="E9" s="2">
-        <v>2267.9800915412302</v>
+        <v>0</v>
       </c>
       <c r="G9">
         <v>5.0000000000000001E-3</v>
@@ -972,10 +972,10 @@
         <v>1</v>
       </c>
       <c r="I9" s="2">
-        <v>937.265745257155</v>
+        <v>1817.2135735827901</v>
       </c>
       <c r="J9" s="2">
-        <v>1749.12202990786</v>
+        <v>0</v>
       </c>
       <c r="L9">
         <v>5.0000000000000001E-3</v>
@@ -984,10 +984,10 @@
         <v>1</v>
       </c>
       <c r="N9" s="2">
-        <v>2102.5930184489998</v>
+        <v>1822.7283052140699</v>
       </c>
       <c r="O9" s="2">
-        <v>2135.3329007505599</v>
+        <v>0</v>
       </c>
       <c r="Q9">
         <v>5.0000000000000001E-3</v>
@@ -996,24 +996,24 @@
         <v>1</v>
       </c>
       <c r="S9" s="2">
-        <v>1258.7168241127199</v>
+        <v>1901.9968061663101</v>
       </c>
       <c r="T9" s="2">
-        <v>1958.6657268086201</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="2:20" x14ac:dyDescent="0.55000000000000004">
       <c r="B10">
-        <v>1</v>
+        <v>1E-3</v>
       </c>
       <c r="C10">
-        <v>1E-3</v>
+        <v>1</v>
       </c>
       <c r="D10" s="2">
-        <v>2098.0196519852898</v>
+        <v>1688.10070322158</v>
       </c>
       <c r="E10" s="2">
-        <v>2098.0196519852898</v>
+        <v>0</v>
       </c>
       <c r="G10">
         <v>1E-3</v>
@@ -1022,10 +1022,10 @@
         <v>1</v>
       </c>
       <c r="I10" s="2">
-        <v>1118.64499942516</v>
+        <v>1734.21819535281</v>
       </c>
       <c r="J10" s="2">
-        <v>1907.5836952679499</v>
+        <v>0</v>
       </c>
       <c r="L10">
         <v>1E-3</v>
@@ -1034,10 +1034,10 @@
         <v>1</v>
       </c>
       <c r="N10" s="2">
-        <v>2186.2723949259998</v>
+        <v>1776.4662402389299</v>
       </c>
       <c r="O10" s="2">
-        <v>2338.7748542782701</v>
+        <v>0</v>
       </c>
       <c r="Q10">
         <v>1E-3</v>
@@ -1046,24 +1046,24 @@
         <v>1</v>
       </c>
       <c r="S10" s="2">
-        <v>1019.81019685212</v>
+        <v>1970.7990690317599</v>
       </c>
       <c r="T10" s="2">
-        <v>1924.1654839571099</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="2:20" x14ac:dyDescent="0.55000000000000004">
       <c r="B11">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="C11">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="D11" s="2">
-        <v>2499.6112055397798</v>
+        <v>0</v>
       </c>
       <c r="E11" s="2">
-        <v>2599.5864599095898</v>
+        <v>0</v>
       </c>
       <c r="G11">
         <v>1</v>
@@ -1072,10 +1072,10 @@
         <v>0.5</v>
       </c>
       <c r="I11" s="2">
-        <v>1242.3308239184501</v>
+        <v>0</v>
       </c>
       <c r="J11" s="2">
-        <v>1969.5135852803401</v>
+        <v>0</v>
       </c>
       <c r="L11">
         <v>1</v>
@@ -1084,10 +1084,10 @@
         <v>0.5</v>
       </c>
       <c r="N11" s="2">
-        <v>1974.2083175493201</v>
+        <v>0</v>
       </c>
       <c r="O11" s="2">
-        <v>2115.5797633058701</v>
+        <v>1842.1837407123501</v>
       </c>
       <c r="Q11">
         <v>1</v>
@@ -1096,10 +1096,10 @@
         <v>0.5</v>
       </c>
       <c r="S11" s="2">
-        <v>1047.5900273402101</v>
+        <v>0</v>
       </c>
       <c r="T11" s="2">
-        <v>2139.1114102729198</v>
+        <v>202.68990830557399</v>
       </c>
     </row>
     <row r="12" spans="2:20" x14ac:dyDescent="0.55000000000000004">
@@ -1110,10 +1110,10 @@
         <v>0.5</v>
       </c>
       <c r="D12" s="2">
-        <v>1901.1557712388901</v>
+        <v>0</v>
       </c>
       <c r="E12" s="2">
-        <v>2051.6463568251802</v>
+        <v>0</v>
       </c>
       <c r="G12">
         <v>0.5</v>
@@ -1122,10 +1122,10 @@
         <v>0.5</v>
       </c>
       <c r="I12" s="2">
-        <v>1048.8832974929801</v>
+        <v>0</v>
       </c>
       <c r="J12" s="2">
-        <v>1764.9991390371699</v>
+        <v>0</v>
       </c>
       <c r="L12">
         <v>0.5</v>
@@ -1134,10 +1134,10 @@
         <v>0.5</v>
       </c>
       <c r="N12" s="2">
-        <v>2364.1669829423299</v>
+        <v>0</v>
       </c>
       <c r="O12" s="2">
-        <v>2429.7189779669702</v>
+        <v>2389.0100540627</v>
       </c>
       <c r="Q12">
         <v>0.5</v>
@@ -1146,24 +1146,24 @@
         <v>0.5</v>
       </c>
       <c r="S12" s="2">
-        <v>731.95433148311804</v>
+        <v>0</v>
       </c>
       <c r="T12" s="2">
-        <v>1938.1343818794701</v>
+        <v>275.45246069986302</v>
       </c>
     </row>
     <row r="13" spans="2:20" x14ac:dyDescent="0.55000000000000004">
       <c r="B13">
-        <v>0.5</v>
+        <v>0.2</v>
       </c>
       <c r="C13">
-        <v>0.2</v>
+        <v>0.5</v>
       </c>
       <c r="D13" s="2">
-        <v>2066.3769132779798</v>
+        <v>1754.7658721038499</v>
       </c>
       <c r="E13" s="2">
-        <v>2200.2394832964401</v>
+        <v>0</v>
       </c>
       <c r="G13">
         <v>0.2</v>
@@ -1172,10 +1172,10 @@
         <v>0.5</v>
       </c>
       <c r="I13" s="2">
-        <v>1082.49665083573</v>
+        <v>0</v>
       </c>
       <c r="J13" s="2">
-        <v>1832.32422138115</v>
+        <v>0</v>
       </c>
       <c r="L13">
         <v>0.2</v>
@@ -1184,10 +1184,10 @@
         <v>0.5</v>
       </c>
       <c r="N13" s="2">
-        <v>2083.33359933464</v>
+        <v>1811.7985341313099</v>
       </c>
       <c r="O13" s="2">
-        <v>2083.33359933464</v>
+        <v>1913.2414332052799</v>
       </c>
       <c r="Q13">
         <v>0.2</v>
@@ -1196,24 +1196,24 @@
         <v>0.5</v>
       </c>
       <c r="S13" s="2">
-        <v>1197.4653968370001</v>
+        <v>315.01279961052398</v>
       </c>
       <c r="T13" s="2">
-        <v>2251.7744778414199</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="2:20" x14ac:dyDescent="0.55000000000000004">
       <c r="B14">
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
       <c r="C14">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
       <c r="D14" s="2">
-        <v>1834.04557794783</v>
+        <v>2069.0995554153401</v>
       </c>
       <c r="E14" s="2">
-        <v>1834.04557794783</v>
+        <v>0</v>
       </c>
       <c r="G14">
         <v>0.1</v>
@@ -1222,10 +1222,10 @@
         <v>0.5</v>
       </c>
       <c r="I14" s="2">
-        <v>813.97335303994998</v>
+        <v>1522.9394689417099</v>
       </c>
       <c r="J14" s="2">
-        <v>1810.4288815996599</v>
+        <v>0</v>
       </c>
       <c r="L14">
         <v>0.1</v>
@@ -1234,10 +1234,10 @@
         <v>0.5</v>
       </c>
       <c r="N14" s="2">
-        <v>2078.10952832253</v>
+        <v>1838.27704805554</v>
       </c>
       <c r="O14" s="2">
-        <v>2142.9276056807798</v>
+        <v>2108.4744578311702</v>
       </c>
       <c r="Q14">
         <v>0.1</v>
@@ -1246,24 +1246,24 @@
         <v>0.5</v>
       </c>
       <c r="S14" s="2">
-        <v>1204.8446041209299</v>
+        <v>1843.25010776832</v>
       </c>
       <c r="T14" s="2">
-        <v>1978.61699479201</v>
+        <v>351.50907054785802</v>
       </c>
     </row>
     <row r="15" spans="2:20" x14ac:dyDescent="0.55000000000000004">
       <c r="B15">
-        <v>0.5</v>
+        <v>0.05</v>
       </c>
       <c r="C15">
-        <v>0.05</v>
+        <v>0.5</v>
       </c>
       <c r="D15" s="2">
-        <v>2233.4083095569999</v>
+        <v>1884.6993504223101</v>
       </c>
       <c r="E15" s="2">
-        <v>2443.3393878485199</v>
+        <v>0</v>
       </c>
       <c r="G15">
         <v>0.05</v>
@@ -1272,10 +1272,10 @@
         <v>0.5</v>
       </c>
       <c r="I15" s="2">
-        <v>871.69103964189003</v>
+        <v>1182.4490826804699</v>
       </c>
       <c r="J15" s="2">
-        <v>2037.5898314034</v>
+        <v>0</v>
       </c>
       <c r="L15">
         <v>0.05</v>
@@ -1284,10 +1284,10 @@
         <v>0.5</v>
       </c>
       <c r="N15" s="2">
-        <v>2247.2691575681501</v>
+        <v>1960.2884586913699</v>
       </c>
       <c r="O15" s="2">
-        <v>2425.0632632080101</v>
+        <v>2105.73101402672</v>
       </c>
       <c r="Q15">
         <v>0.05</v>
@@ -1296,24 +1296,24 @@
         <v>0.5</v>
       </c>
       <c r="S15" s="2">
-        <v>771.49909230251899</v>
+        <v>1697.7489510385501</v>
       </c>
       <c r="T15" s="2">
-        <v>2085.7610952865198</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="2:20" x14ac:dyDescent="0.55000000000000004">
       <c r="B16">
-        <v>0.5</v>
+        <v>0.01</v>
       </c>
       <c r="C16">
-        <v>0.01</v>
+        <v>0.5</v>
       </c>
       <c r="D16" s="2">
-        <v>2000.8758966481</v>
+        <v>1803.9006853012099</v>
       </c>
       <c r="E16" s="2">
-        <v>2200.9612190990701</v>
+        <v>0</v>
       </c>
       <c r="G16">
         <v>0.01</v>
@@ -1322,10 +1322,10 @@
         <v>0.5</v>
       </c>
       <c r="I16" s="2">
-        <v>1064.6256958952899</v>
+        <v>1471.34559899233</v>
       </c>
       <c r="J16" s="2">
-        <v>1896.23397375691</v>
+        <v>0</v>
       </c>
       <c r="L16">
         <v>0.01</v>
@@ -1334,10 +1334,10 @@
         <v>0.5</v>
       </c>
       <c r="N16" s="2">
-        <v>2414.7568281992399</v>
+        <v>2277.5007157047899</v>
       </c>
       <c r="O16" s="2">
-        <v>2514.0488615169702</v>
+        <v>2453.0452245246001</v>
       </c>
       <c r="Q16">
         <v>0.01</v>
@@ -1346,24 +1346,24 @@
         <v>0.5</v>
       </c>
       <c r="S16" s="2">
-        <v>1079.8943668356701</v>
+        <v>1846.1282347772999</v>
       </c>
       <c r="T16" s="2">
-        <v>2007.2867197591199</v>
+        <v>318.04394476259603</v>
       </c>
     </row>
     <row r="17" spans="2:20" x14ac:dyDescent="0.55000000000000004">
       <c r="B17">
-        <v>0.5</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="C17">
-        <v>5.0000000000000001E-3</v>
+        <v>0.5</v>
       </c>
       <c r="D17" s="2">
-        <v>2235.30337745099</v>
+        <v>2078.4308952393999</v>
       </c>
       <c r="E17" s="2">
-        <v>2404.9131390713801</v>
+        <v>0</v>
       </c>
       <c r="G17">
         <v>5.0000000000000001E-3</v>
@@ -1372,10 +1372,10 @@
         <v>0.5</v>
       </c>
       <c r="I17" s="2">
-        <v>767.03155645080199</v>
+        <v>2014.16878099766</v>
       </c>
       <c r="J17" s="2">
-        <v>1919.55165007751</v>
+        <v>0</v>
       </c>
       <c r="L17">
         <v>5.0000000000000001E-3</v>
@@ -1384,10 +1384,10 @@
         <v>0.5</v>
       </c>
       <c r="N17" s="2">
-        <v>2351.1155234929602</v>
+        <v>1755.4324084508601</v>
       </c>
       <c r="O17" s="2">
-        <v>2403.4790705629698</v>
+        <v>1764.3266476768599</v>
       </c>
       <c r="Q17">
         <v>5.0000000000000001E-3</v>
@@ -1396,24 +1396,24 @@
         <v>0.5</v>
       </c>
       <c r="S17" s="2">
-        <v>992.78337801332896</v>
+        <v>1984.6118347813799</v>
       </c>
       <c r="T17" s="2">
-        <v>1928.7750178802301</v>
+        <v>289.84990194267601</v>
       </c>
     </row>
     <row r="18" spans="2:20" x14ac:dyDescent="0.55000000000000004">
       <c r="B18">
-        <v>0.5</v>
+        <v>1E-3</v>
       </c>
       <c r="C18">
-        <v>1E-3</v>
+        <v>0.5</v>
       </c>
       <c r="D18" s="2">
-        <v>2081.3750778797798</v>
+        <v>1947.79583328688</v>
       </c>
       <c r="E18" s="2">
-        <v>2142.2641709260402</v>
+        <v>0</v>
       </c>
       <c r="G18">
         <v>1E-3</v>
@@ -1422,10 +1422,10 @@
         <v>0.5</v>
       </c>
       <c r="I18" s="2">
-        <v>999.89630084719602</v>
+        <v>1824.8040391910699</v>
       </c>
       <c r="J18" s="2">
-        <v>2053.1187224239002</v>
+        <v>0</v>
       </c>
       <c r="L18">
         <v>1E-3</v>
@@ -1434,10 +1434,10 @@
         <v>0.5</v>
       </c>
       <c r="N18" s="2">
-        <v>2011.7130643042001</v>
+        <v>1890.4135154628</v>
       </c>
       <c r="O18" s="2">
-        <v>2011.7130643042001</v>
+        <v>1890.4135154628</v>
       </c>
       <c r="Q18">
         <v>1E-3</v>
@@ -1446,24 +1446,24 @@
         <v>0.5</v>
       </c>
       <c r="S18" s="2">
-        <v>1256.8201560535799</v>
+        <v>1985.7994219360701</v>
       </c>
       <c r="T18" s="2">
-        <v>1903.0718151506701</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="2:20" x14ac:dyDescent="0.55000000000000004">
       <c r="B19">
-        <v>0.2</v>
+        <v>1</v>
       </c>
       <c r="C19">
-        <v>1</v>
+        <v>0.2</v>
       </c>
       <c r="D19" s="2">
-        <v>2082.5060806880501</v>
+        <v>0</v>
       </c>
       <c r="E19" s="2">
-        <v>2157.8429858772201</v>
+        <v>1989.74432766731</v>
       </c>
       <c r="G19">
         <v>1</v>
@@ -1472,10 +1472,10 @@
         <v>0.2</v>
       </c>
       <c r="I19" s="2">
-        <v>891.26179929765397</v>
+        <v>0</v>
       </c>
       <c r="J19" s="2">
-        <v>1874.91407013196</v>
+        <v>78.940582530916998</v>
       </c>
       <c r="L19">
         <v>1</v>
@@ -1484,10 +1484,10 @@
         <v>0.2</v>
       </c>
       <c r="N19" s="2">
-        <v>2235.9529145043998</v>
+        <v>0</v>
       </c>
       <c r="O19" s="2">
-        <v>2387.7768725208498</v>
+        <v>1863.42895523164</v>
       </c>
       <c r="Q19">
         <v>1</v>
@@ -1496,24 +1496,24 @@
         <v>0.2</v>
       </c>
       <c r="S19" s="2">
-        <v>544.30149533742804</v>
+        <v>0</v>
       </c>
       <c r="T19" s="2">
-        <v>1871.81473929188</v>
+        <v>2129.4688885268502</v>
       </c>
     </row>
     <row r="20" spans="2:20" x14ac:dyDescent="0.55000000000000004">
       <c r="B20">
-        <v>0.2</v>
+        <v>0.5</v>
       </c>
       <c r="C20">
-        <v>0.5</v>
+        <v>0.2</v>
       </c>
       <c r="D20" s="2">
-        <v>2264.9135740914699</v>
+        <v>0</v>
       </c>
       <c r="E20" s="2">
-        <v>2334.0560728752098</v>
+        <v>1859.1061274364399</v>
       </c>
       <c r="G20">
         <v>0.5</v>
@@ -1522,10 +1522,10 @@
         <v>0.2</v>
       </c>
       <c r="I20" s="2">
-        <v>1293.54520770612</v>
+        <v>0</v>
       </c>
       <c r="J20" s="2">
-        <v>2003.62758179463</v>
+        <v>74.706935248917603</v>
       </c>
       <c r="L20">
         <v>0.5</v>
@@ -1534,10 +1534,10 @@
         <v>0.2</v>
       </c>
       <c r="N20" s="2">
-        <v>2226.4070135911402</v>
+        <v>0</v>
       </c>
       <c r="O20" s="2">
-        <v>2226.4070135911402</v>
+        <v>2146.7841141004201</v>
       </c>
       <c r="Q20">
         <v>0.5</v>
@@ -1546,10 +1546,10 @@
         <v>0.2</v>
       </c>
       <c r="S20" s="2">
-        <v>997.86534772965001</v>
+        <v>0</v>
       </c>
       <c r="T20" s="2">
-        <v>2015.5158553118599</v>
+        <v>1792.8239776448099</v>
       </c>
     </row>
     <row r="21" spans="2:20" x14ac:dyDescent="0.55000000000000004">
@@ -1560,10 +1560,10 @@
         <v>0.2</v>
       </c>
       <c r="D21" s="2">
-        <v>2361.9240174902202</v>
+        <v>1924.9650934061899</v>
       </c>
       <c r="E21" s="2">
-        <v>2590.24626771567</v>
+        <v>2227.33316670967</v>
       </c>
       <c r="G21">
         <v>0.2</v>
@@ -1572,10 +1572,10 @@
         <v>0.2</v>
       </c>
       <c r="I21" s="2">
-        <v>1016.14575172772</v>
+        <v>0</v>
       </c>
       <c r="J21" s="2">
-        <v>1705.68923790023</v>
+        <v>181.58841206989999</v>
       </c>
       <c r="L21">
         <v>0.2</v>
@@ -1584,10 +1584,10 @@
         <v>0.2</v>
       </c>
       <c r="N21" s="2">
-        <v>2279.5838086389399</v>
+        <v>1925.75205768208</v>
       </c>
       <c r="O21" s="2">
-        <v>2370.8625498354399</v>
+        <v>1973.49250467395</v>
       </c>
       <c r="Q21">
         <v>0.2</v>
@@ -1596,24 +1596,24 @@
         <v>0.2</v>
       </c>
       <c r="S21" s="2">
-        <v>896.55437465752698</v>
+        <v>511.02676429606203</v>
       </c>
       <c r="T21" s="2">
-        <v>1900.58094332836</v>
+        <v>1906.5130300138101</v>
       </c>
     </row>
     <row r="22" spans="2:20" x14ac:dyDescent="0.55000000000000004">
       <c r="B22">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="C22">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="D22" s="2">
-        <v>2077.3907508930602</v>
+        <v>1758.80166741938</v>
       </c>
       <c r="E22" s="2">
-        <v>2092.0763413918698</v>
+        <v>1760.1843009337899</v>
       </c>
       <c r="G22">
         <v>0.1</v>
@@ -1622,10 +1622,10 @@
         <v>0.2</v>
       </c>
       <c r="I22" s="2">
-        <v>835.47118309668497</v>
+        <v>1056.36308724843</v>
       </c>
       <c r="J22" s="2">
-        <v>1638.1753281184499</v>
+        <v>0</v>
       </c>
       <c r="L22">
         <v>0.1</v>
@@ -1634,10 +1634,10 @@
         <v>0.2</v>
       </c>
       <c r="N22" s="2">
-        <v>1860.60210708055</v>
+        <v>1829.5809639776101</v>
       </c>
       <c r="O22" s="2">
-        <v>2003.6392248422901</v>
+        <v>1959.40348035289</v>
       </c>
       <c r="Q22">
         <v>0.1</v>
@@ -1646,24 +1646,24 @@
         <v>0.2</v>
       </c>
       <c r="S22" s="2">
-        <v>1088.34028476705</v>
+        <v>1884.73372163414</v>
       </c>
       <c r="T22" s="2">
-        <v>1788.28903000079</v>
+        <v>1814.65781693587</v>
       </c>
     </row>
     <row r="23" spans="2:20" x14ac:dyDescent="0.55000000000000004">
       <c r="B23">
-        <v>0.2</v>
+        <v>0.05</v>
       </c>
       <c r="C23">
-        <v>0.05</v>
+        <v>0.2</v>
       </c>
       <c r="D23" s="2">
-        <v>2091.92422951352</v>
+        <v>2218.0890359125701</v>
       </c>
       <c r="E23" s="2">
-        <v>2125.1919894089801</v>
+        <v>2167.7160830233802</v>
       </c>
       <c r="G23">
         <v>0.05</v>
@@ -1672,10 +1672,10 @@
         <v>0.2</v>
       </c>
       <c r="I23" s="2">
-        <v>1201.2728388299599</v>
+        <v>1216.74189715069</v>
       </c>
       <c r="J23" s="2">
-        <v>1602.12816183474</v>
+        <v>97.020740175976698</v>
       </c>
       <c r="L23">
         <v>0.05</v>
@@ -1684,10 +1684,10 @@
         <v>0.2</v>
       </c>
       <c r="N23" s="2">
-        <v>2247.17246591608</v>
+        <v>2064.7836159450098</v>
       </c>
       <c r="O23" s="2">
-        <v>2328.6333680037601</v>
+        <v>2214.6345593076999</v>
       </c>
       <c r="Q23">
         <v>0.05</v>
@@ -1696,24 +1696,24 @@
         <v>0.2</v>
       </c>
       <c r="S23" s="2">
-        <v>607.72412241643497</v>
+        <v>1796.8365529488799</v>
       </c>
       <c r="T23" s="2">
-        <v>2139.7664344597301</v>
+        <v>1796.8365529488799</v>
       </c>
     </row>
     <row r="24" spans="2:20" x14ac:dyDescent="0.55000000000000004">
       <c r="B24">
-        <v>0.2</v>
+        <v>0.01</v>
       </c>
       <c r="C24">
-        <v>0.01</v>
+        <v>0.2</v>
       </c>
       <c r="D24" s="2">
-        <v>1970.19755520579</v>
+        <v>2099.36068740583</v>
       </c>
       <c r="E24" s="2">
-        <v>2054.6821200629602</v>
+        <v>2217.8936413760298</v>
       </c>
       <c r="G24">
         <v>0.01</v>
@@ -1722,10 +1722,10 @@
         <v>0.2</v>
       </c>
       <c r="I24" s="2">
-        <v>1247.27659265631</v>
+        <v>1541.5299843483101</v>
       </c>
       <c r="J24" s="2">
-        <v>2126.4650401590802</v>
+        <v>181.66549237631</v>
       </c>
       <c r="L24">
         <v>0.01</v>
@@ -1734,10 +1734,10 @@
         <v>0.2</v>
       </c>
       <c r="N24" s="2">
-        <v>2003.15648099193</v>
+        <v>1810.7760254062</v>
       </c>
       <c r="O24" s="2">
-        <v>2003.15648099193</v>
+        <v>1975.1918096536899</v>
       </c>
       <c r="Q24">
         <v>0.01</v>
@@ -1746,24 +1746,24 @@
         <v>0.2</v>
       </c>
       <c r="S24" s="2">
-        <v>952.06073944125296</v>
+        <v>1989.4310200575001</v>
       </c>
       <c r="T24" s="2">
-        <v>1677.8043410591699</v>
+        <v>1982.5861194822601</v>
       </c>
     </row>
     <row r="25" spans="2:20" x14ac:dyDescent="0.55000000000000004">
       <c r="B25">
-        <v>0.2</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="C25">
-        <v>5.0000000000000001E-3</v>
+        <v>0.2</v>
       </c>
       <c r="D25" s="2">
-        <v>1996.0158685797401</v>
+        <v>1785.16344472487</v>
       </c>
       <c r="E25" s="2">
-        <v>2060.50455357082</v>
+        <v>1799.79440028149</v>
       </c>
       <c r="G25">
         <v>5.0000000000000001E-3</v>
@@ -1772,10 +1772,10 @@
         <v>0.2</v>
       </c>
       <c r="I25" s="2">
-        <v>899.63449517748995</v>
+        <v>1575.3778339155799</v>
       </c>
       <c r="J25" s="2">
-        <v>1712.9753568292599</v>
+        <v>189.538338226501</v>
       </c>
       <c r="L25">
         <v>5.0000000000000001E-3</v>
@@ -1784,10 +1784,10 @@
         <v>0.2</v>
       </c>
       <c r="N25" s="2">
-        <v>2262.7647975064201</v>
+        <v>1922.4415137475501</v>
       </c>
       <c r="O25" s="2">
-        <v>2360.3173524567001</v>
+        <v>1942.04043048482</v>
       </c>
       <c r="Q25">
         <v>5.0000000000000001E-3</v>
@@ -1796,24 +1796,24 @@
         <v>0.2</v>
       </c>
       <c r="S25" s="2">
-        <v>1134.47349006373</v>
+        <v>1676.56624130153</v>
       </c>
       <c r="T25" s="2">
-        <v>2033.4007691772699</v>
+        <v>1526.56624130153</v>
       </c>
     </row>
     <row r="26" spans="2:20" x14ac:dyDescent="0.55000000000000004">
       <c r="B26">
-        <v>0.2</v>
+        <v>1E-3</v>
       </c>
       <c r="C26">
-        <v>1E-3</v>
+        <v>0.2</v>
       </c>
       <c r="D26" s="2">
-        <v>2087.0647226239798</v>
+        <v>1854.2794190597299</v>
       </c>
       <c r="E26" s="2">
-        <v>2195.9543346693199</v>
+        <v>1886.90048592121</v>
       </c>
       <c r="G26">
         <v>1E-3</v>
@@ -1822,10 +1822,10 @@
         <v>0.2</v>
       </c>
       <c r="I26" s="2">
-        <v>703.90982305576597</v>
+        <v>1884.8263364289201</v>
       </c>
       <c r="J26" s="2">
-        <v>1681.54664572242</v>
+        <v>87.974306547856003</v>
       </c>
       <c r="L26">
         <v>1E-3</v>
@@ -1834,10 +1834,10 @@
         <v>0.2</v>
       </c>
       <c r="N26" s="2">
-        <v>2113.51637340856</v>
+        <v>1657.5146567230199</v>
       </c>
       <c r="O26" s="2">
-        <v>2230.9649590208301</v>
+        <v>1670.8090382099101</v>
       </c>
       <c r="Q26">
         <v>1E-3</v>
@@ -1846,24 +1846,24 @@
         <v>0.2</v>
       </c>
       <c r="S26" s="2">
-        <v>976.64735393046499</v>
+        <v>2077.4484728849902</v>
       </c>
       <c r="T26" s="2">
-        <v>2049.3583495385101</v>
+        <v>2081.1881192739902</v>
       </c>
     </row>
     <row r="27" spans="2:20" x14ac:dyDescent="0.55000000000000004">
       <c r="B27">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="C27">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="D27" s="2">
-        <v>2194.8160500733502</v>
+        <v>0</v>
       </c>
       <c r="E27" s="2">
-        <v>2423.5223675782299</v>
+        <v>2173.62085634508</v>
       </c>
       <c r="G27">
         <v>1</v>
@@ -1872,10 +1872,10 @@
         <v>0.1</v>
       </c>
       <c r="I27" s="2">
-        <v>1165.1895308620001</v>
+        <v>0</v>
       </c>
       <c r="J27" s="2">
-        <v>1704.254890441</v>
+        <v>1020.00958427921</v>
       </c>
       <c r="L27">
         <v>1</v>
@@ -1884,10 +1884,10 @@
         <v>0.1</v>
       </c>
       <c r="N27" s="2">
-        <v>1832.9238296518299</v>
+        <v>0</v>
       </c>
       <c r="O27" s="2">
-        <v>1941.4353335972201</v>
+        <v>2011.5008555511499</v>
       </c>
       <c r="Q27">
         <v>1</v>
@@ -1896,24 +1896,24 @@
         <v>0.1</v>
       </c>
       <c r="S27" s="2">
-        <v>641.27467627869999</v>
+        <v>0</v>
       </c>
       <c r="T27" s="2">
-        <v>1776.1780060265601</v>
+        <v>1832.0108045371301</v>
       </c>
     </row>
     <row r="28" spans="2:20" x14ac:dyDescent="0.55000000000000004">
       <c r="B28">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
       <c r="C28">
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
       <c r="D28" s="2">
-        <v>2055.05683244889</v>
+        <v>0</v>
       </c>
       <c r="E28" s="2">
-        <v>2087.2227506234099</v>
+        <v>2100.4894370673501</v>
       </c>
       <c r="G28">
         <v>0.5</v>
@@ -1922,10 +1922,10 @@
         <v>0.1</v>
       </c>
       <c r="I28" s="2">
-        <v>1262.1857843734699</v>
+        <v>0</v>
       </c>
       <c r="J28" s="2">
-        <v>1960.51793529159</v>
+        <v>1103.21083315429</v>
       </c>
       <c r="L28">
         <v>0.5</v>
@@ -1934,10 +1934,10 @@
         <v>0.1</v>
       </c>
       <c r="N28" s="2">
-        <v>2430.1812714091998</v>
+        <v>0</v>
       </c>
       <c r="O28" s="2">
-        <v>2442.4452884810198</v>
+        <v>1978.29924534918</v>
       </c>
       <c r="Q28">
         <v>0.5</v>
@@ -1946,24 +1946,24 @@
         <v>0.1</v>
       </c>
       <c r="S28" s="2">
-        <v>1042.35718081906</v>
+        <v>0</v>
       </c>
       <c r="T28" s="2">
-        <v>1825.34354216257</v>
+        <v>1831.0159791410999</v>
       </c>
     </row>
     <row r="29" spans="2:20" x14ac:dyDescent="0.55000000000000004">
       <c r="B29">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="C29">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="D29" s="2">
-        <v>2195.1401248150701</v>
+        <v>1812.6562676012099</v>
       </c>
       <c r="E29" s="2">
-        <v>2222.4371720495001</v>
+        <v>1915.7515387702099</v>
       </c>
       <c r="G29">
         <v>0.2</v>
@@ -1972,10 +1972,10 @@
         <v>0.1</v>
       </c>
       <c r="I29" s="2">
-        <v>892.52927287532805</v>
+        <v>0</v>
       </c>
       <c r="J29" s="2">
-        <v>1872.17630443448</v>
+        <v>1244.12671434053</v>
       </c>
       <c r="L29">
         <v>0.2</v>
@@ -1984,10 +1984,10 @@
         <v>0.1</v>
       </c>
       <c r="N29" s="2">
-        <v>2092.2285787969799</v>
+        <v>1784.8432802781899</v>
       </c>
       <c r="O29" s="2">
-        <v>2199.4077762882798</v>
+        <v>1816.1643213999801</v>
       </c>
       <c r="Q29">
         <v>0.2</v>
@@ -1996,10 +1996,10 @@
         <v>0.1</v>
       </c>
       <c r="S29" s="2">
-        <v>1010.58811875375</v>
+        <v>319.33837661331103</v>
       </c>
       <c r="T29" s="2">
-        <v>1849.2943934756299</v>
+        <v>1698.3548042151299</v>
       </c>
     </row>
     <row r="30" spans="2:20" x14ac:dyDescent="0.55000000000000004">
@@ -2010,10 +2010,10 @@
         <v>0.1</v>
       </c>
       <c r="D30" s="2">
-        <v>2059.0890565012601</v>
+        <v>1767.6496223245099</v>
       </c>
       <c r="E30" s="2">
-        <v>2059.0890565012601</v>
+        <v>1987.5659211889199</v>
       </c>
       <c r="G30">
         <v>0.1</v>
@@ -2022,10 +2022,10 @@
         <v>0.1</v>
       </c>
       <c r="I30" s="2">
-        <v>1058.44579783885</v>
+        <v>742.03833221343598</v>
       </c>
       <c r="J30" s="2">
-        <v>1633.39292321981</v>
+        <v>1048.81763916523</v>
       </c>
       <c r="L30">
         <v>0.1</v>
@@ -2034,10 +2034,10 @@
         <v>0.1</v>
       </c>
       <c r="N30" s="2">
-        <v>2073.0810034204401</v>
+        <v>2001.4539636503</v>
       </c>
       <c r="O30" s="2">
-        <v>2247.0979442254402</v>
+        <v>2100.6236837947099</v>
       </c>
       <c r="Q30">
         <v>0.1</v>
@@ -2046,24 +2046,24 @@
         <v>0.1</v>
       </c>
       <c r="S30" s="2">
-        <v>960.37054981237998</v>
+        <v>1644.0003433473601</v>
       </c>
       <c r="T30" s="2">
-        <v>1659.7975228631201</v>
+        <v>2329.951916431</v>
       </c>
     </row>
     <row r="31" spans="2:20" x14ac:dyDescent="0.55000000000000004">
       <c r="B31">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="C31">
-        <v>0.05</v>
+        <v>0.1</v>
       </c>
       <c r="D31" s="2">
-        <v>2067.9370224884401</v>
+        <v>1809.81556069369</v>
       </c>
       <c r="E31" s="2">
-        <v>2161.17715268336</v>
+        <v>1993.6980278579899</v>
       </c>
       <c r="G31">
         <v>0.05</v>
@@ -2072,10 +2072,10 @@
         <v>0.1</v>
       </c>
       <c r="I31" s="2">
-        <v>909.80506972648595</v>
+        <v>1109.2361095373301</v>
       </c>
       <c r="J31" s="2">
-        <v>1822.8315442289399</v>
+        <v>1137.9263820035101</v>
       </c>
       <c r="L31">
         <v>0.05</v>
@@ -2084,10 +2084,10 @@
         <v>0.1</v>
       </c>
       <c r="N31" s="2">
-        <v>2420.50834179702</v>
+        <v>2309.1486254121301</v>
       </c>
       <c r="O31" s="2">
-        <v>2540.4675802151801</v>
+        <v>2484.5990547111001</v>
       </c>
       <c r="Q31">
         <v>0.05</v>
@@ -2096,24 +2096,24 @@
         <v>0.1</v>
       </c>
       <c r="S31" s="2">
-        <v>898.18529171937905</v>
+        <v>1885.2642723132101</v>
       </c>
       <c r="T31" s="2">
-        <v>1757.0598367801699</v>
+        <v>1986.05608711541</v>
       </c>
     </row>
     <row r="32" spans="2:20" x14ac:dyDescent="0.55000000000000004">
       <c r="B32">
-        <v>0.1</v>
+        <v>0.01</v>
       </c>
       <c r="C32">
-        <v>0.01</v>
+        <v>0.1</v>
       </c>
       <c r="D32" s="2">
-        <v>2352.4186936420601</v>
+        <v>2261.3286243838702</v>
       </c>
       <c r="E32" s="2">
-        <v>2380.7551160857402</v>
+        <v>2280.9290700085098</v>
       </c>
       <c r="G32">
         <v>0.01</v>
@@ -2122,10 +2122,10 @@
         <v>0.1</v>
       </c>
       <c r="I32" s="2">
-        <v>1425.60030030948</v>
+        <v>1665.7725536871601</v>
       </c>
       <c r="J32" s="2">
-        <v>2129.0637867690698</v>
+        <v>1040.9882914396801</v>
       </c>
       <c r="L32">
         <v>0.01</v>
@@ -2134,10 +2134,10 @@
         <v>0.1</v>
       </c>
       <c r="N32" s="2">
-        <v>2465.0761957109698</v>
+        <v>2020.1316297298999</v>
       </c>
       <c r="O32" s="2">
-        <v>2646.4026635565801</v>
+        <v>2202.4566164124799</v>
       </c>
       <c r="Q32">
         <v>0.01</v>
@@ -2146,24 +2146,24 @@
         <v>0.1</v>
       </c>
       <c r="S32" s="2">
-        <v>1144.7525459517101</v>
+        <v>2320.0197192097098</v>
       </c>
       <c r="T32" s="2">
-        <v>2045.0876779673899</v>
+        <v>2375.2665253492601</v>
       </c>
     </row>
     <row r="33" spans="2:20" x14ac:dyDescent="0.55000000000000004">
       <c r="B33">
-        <v>0.1</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="C33">
-        <v>5.0000000000000001E-3</v>
+        <v>0.1</v>
       </c>
       <c r="D33" s="2">
-        <v>2356.6413066209798</v>
+        <v>2342.88820511833</v>
       </c>
       <c r="E33" s="2">
-        <v>2534.39021593288</v>
+        <v>2377.4111757328001</v>
       </c>
       <c r="G33">
         <v>5.0000000000000001E-3</v>
@@ -2172,10 +2172,10 @@
         <v>0.1</v>
       </c>
       <c r="I33" s="2">
-        <v>1130.43493647675</v>
+        <v>1743.10750650367</v>
       </c>
       <c r="J33" s="2">
-        <v>1780.97232060183</v>
+        <v>993.33389263768299</v>
       </c>
       <c r="L33">
         <v>5.0000000000000001E-3</v>
@@ -2184,10 +2184,10 @@
         <v>0.1</v>
       </c>
       <c r="N33" s="2">
-        <v>2056.2043359623399</v>
+        <v>2269.3672373146801</v>
       </c>
       <c r="O33" s="2">
-        <v>2173.6140996012</v>
+        <v>2440.26373061512</v>
       </c>
       <c r="Q33">
         <v>5.0000000000000001E-3</v>
@@ -2196,24 +2196,24 @@
         <v>0.1</v>
       </c>
       <c r="S33" s="2">
-        <v>1233.80277682322</v>
+        <v>2251.01435479462</v>
       </c>
       <c r="T33" s="2">
-        <v>1753.98588062354</v>
+        <v>2266.0175200609901</v>
       </c>
     </row>
     <row r="34" spans="2:20" x14ac:dyDescent="0.55000000000000004">
       <c r="B34">
-        <v>0.1</v>
+        <v>1E-3</v>
       </c>
       <c r="C34">
-        <v>1E-3</v>
+        <v>0.1</v>
       </c>
       <c r="D34" s="2">
-        <v>1876.77620804761</v>
+        <v>1765.6645407718399</v>
       </c>
       <c r="E34" s="2">
-        <v>2004.51587631339</v>
+        <v>1765.6645407718399</v>
       </c>
       <c r="G34">
         <v>1E-3</v>
@@ -2222,10 +2222,10 @@
         <v>0.1</v>
       </c>
       <c r="I34" s="2">
-        <v>594.95248691238305</v>
+        <v>1709.2400087045901</v>
       </c>
       <c r="J34" s="2">
-        <v>2065.9815525264798</v>
+        <v>1085.4164449559501</v>
       </c>
       <c r="L34">
         <v>1E-3</v>
@@ -2234,10 +2234,10 @@
         <v>0.1</v>
       </c>
       <c r="N34" s="2">
-        <v>2044.4069829264199</v>
+        <v>2421.2476065720698</v>
       </c>
       <c r="O34" s="2">
-        <v>2181.20831015453</v>
+        <v>2421.2476065720698</v>
       </c>
       <c r="Q34">
         <v>1E-3</v>
@@ -2246,24 +2246,24 @@
         <v>0.1</v>
       </c>
       <c r="S34" s="2">
-        <v>583.60873141540901</v>
+        <v>2191.53083925792</v>
       </c>
       <c r="T34" s="2">
-        <v>1916.1714684625299</v>
+        <v>2253.5894235983001</v>
       </c>
     </row>
     <row r="35" spans="2:20" x14ac:dyDescent="0.55000000000000004">
       <c r="B35">
-        <v>0.05</v>
+        <v>1</v>
       </c>
       <c r="C35">
-        <v>1</v>
+        <v>0.05</v>
       </c>
       <c r="D35" s="2">
-        <v>2225.7147547944201</v>
+        <v>0</v>
       </c>
       <c r="E35" s="2">
-        <v>2262.6374126919</v>
+        <v>2044.8160381898099</v>
       </c>
       <c r="G35">
         <v>1</v>
@@ -2272,10 +2272,10 @@
         <v>0.05</v>
       </c>
       <c r="I35" s="2">
-        <v>731.54838082310403</v>
+        <v>0</v>
       </c>
       <c r="J35" s="2">
-        <v>1869.6234742904301</v>
+        <v>1546.13362517002</v>
       </c>
       <c r="L35">
         <v>1</v>
@@ -2284,10 +2284,10 @@
         <v>0.05</v>
       </c>
       <c r="N35" s="2">
-        <v>1853.6673112455301</v>
+        <v>0</v>
       </c>
       <c r="O35" s="2">
-        <v>1990.9138256772201</v>
+        <v>1982.83346763947</v>
       </c>
       <c r="Q35">
         <v>1</v>
@@ -2296,24 +2296,24 @@
         <v>0.05</v>
       </c>
       <c r="S35" s="2">
-        <v>1081.1434285733701</v>
+        <v>0</v>
       </c>
       <c r="T35" s="2">
-        <v>1861.93258760191</v>
+        <v>2159.2894443679002</v>
       </c>
     </row>
     <row r="36" spans="2:20" x14ac:dyDescent="0.55000000000000004">
       <c r="B36">
-        <v>0.05</v>
+        <v>0.5</v>
       </c>
       <c r="C36">
-        <v>0.5</v>
+        <v>0.05</v>
       </c>
       <c r="D36" s="2">
-        <v>2066.3576403584302</v>
+        <v>0</v>
       </c>
       <c r="E36" s="2">
-        <v>2131.0612821370901</v>
+        <v>2138.3434793424499</v>
       </c>
       <c r="G36">
         <v>0.5</v>
@@ -2322,10 +2322,10 @@
         <v>0.05</v>
       </c>
       <c r="I36" s="2">
-        <v>746.816742217914</v>
+        <v>0</v>
       </c>
       <c r="J36" s="2">
-        <v>1737.84041109588</v>
+        <v>1628.3925784861499</v>
       </c>
       <c r="L36">
         <v>0.5</v>
@@ -2334,10 +2334,10 @@
         <v>0.05</v>
       </c>
       <c r="N36" s="2">
-        <v>2077.1129956526302</v>
+        <v>0</v>
       </c>
       <c r="O36" s="2">
-        <v>2116.9523662817901</v>
+        <v>1797.0283366384899</v>
       </c>
       <c r="Q36">
         <v>0.5</v>
@@ -2346,24 +2346,24 @@
         <v>0.05</v>
       </c>
       <c r="S36" s="2">
-        <v>879.525169484196</v>
+        <v>0</v>
       </c>
       <c r="T36" s="2">
-        <v>1800.39575800123</v>
+        <v>1914.6136565582699</v>
       </c>
     </row>
     <row r="37" spans="2:20" x14ac:dyDescent="0.55000000000000004">
       <c r="B37">
-        <v>0.05</v>
+        <v>0.2</v>
       </c>
       <c r="C37">
-        <v>0.2</v>
+        <v>0.05</v>
       </c>
       <c r="D37" s="2">
-        <v>2278.7896406364698</v>
+        <v>1972.8589930103001</v>
       </c>
       <c r="E37" s="2">
-        <v>2320.6058590324901</v>
+        <v>2663.6412610039301</v>
       </c>
       <c r="G37">
         <v>0.2</v>
@@ -2372,10 +2372,10 @@
         <v>0.05</v>
       </c>
       <c r="I37" s="2">
-        <v>1281.97505888925</v>
+        <v>0</v>
       </c>
       <c r="J37" s="2">
-        <v>1915.8150177273001</v>
+        <v>1591.07025581321</v>
       </c>
       <c r="L37">
         <v>0.2</v>
@@ -2384,10 +2384,10 @@
         <v>0.05</v>
       </c>
       <c r="N37" s="2">
-        <v>2264.9226543632299</v>
+        <v>1753.52855094595</v>
       </c>
       <c r="O37" s="2">
-        <v>2289.6677581233798</v>
+        <v>1807.2902710029</v>
       </c>
       <c r="Q37">
         <v>0.2</v>
@@ -2396,24 +2396,24 @@
         <v>0.05</v>
       </c>
       <c r="S37" s="2">
-        <v>1081.55102230224</v>
+        <v>397.39163017096803</v>
       </c>
       <c r="T37" s="2">
-        <v>1817.0803984634499</v>
+        <v>2091.3718594359898</v>
       </c>
     </row>
     <row r="38" spans="2:20" x14ac:dyDescent="0.55000000000000004">
       <c r="B38">
-        <v>0.05</v>
+        <v>0.1</v>
       </c>
       <c r="C38">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="D38" s="2">
-        <v>1930.2002346541201</v>
+        <v>1898.99931462677</v>
       </c>
       <c r="E38" s="2">
-        <v>1968.75900460195</v>
+        <v>1921.2313015448201</v>
       </c>
       <c r="G38">
         <v>0.1</v>
@@ -2422,10 +2422,10 @@
         <v>0.05</v>
       </c>
       <c r="I38" s="2">
-        <v>1274.92231049218</v>
+        <v>1107.92819107891</v>
       </c>
       <c r="J38" s="2">
-        <v>1935.2480198603</v>
+        <v>1604.62492588856</v>
       </c>
       <c r="L38">
         <v>0.1</v>
@@ -2434,10 +2434,10 @@
         <v>0.05</v>
       </c>
       <c r="N38" s="2">
-        <v>1995.2619906074001</v>
+        <v>1839.16771971658</v>
       </c>
       <c r="O38" s="2">
-        <v>2217.68129452413</v>
+        <v>1930.68926354316</v>
       </c>
       <c r="Q38">
         <v>0.1</v>
@@ -2446,10 +2446,10 @@
         <v>0.05</v>
       </c>
       <c r="S38" s="2">
-        <v>1330.7364229552099</v>
+        <v>1975.8760601292299</v>
       </c>
       <c r="T38" s="2">
-        <v>2164.6324243826298</v>
+        <v>2273.74109216537</v>
       </c>
     </row>
     <row r="39" spans="2:20" x14ac:dyDescent="0.55000000000000004">
@@ -2460,10 +2460,10 @@
         <v>0.05</v>
       </c>
       <c r="D39" s="2">
-        <v>1899.9230021368901</v>
+        <v>2284.9296869434502</v>
       </c>
       <c r="E39" s="2">
-        <v>1903.1228529645</v>
+        <v>2437.4869179915199</v>
       </c>
       <c r="G39">
         <v>0.05</v>
@@ -2472,10 +2472,10 @@
         <v>0.05</v>
       </c>
       <c r="I39" s="2">
-        <v>1050.4433580314001</v>
+        <v>1234.3194776755799</v>
       </c>
       <c r="J39" s="2">
-        <v>1788.2775991408</v>
+        <v>2000.7752249391999</v>
       </c>
       <c r="L39">
         <v>0.05</v>
@@ -2484,10 +2484,10 @@
         <v>0.05</v>
       </c>
       <c r="N39" s="2">
-        <v>2031.60891626748</v>
+        <v>2277.4795221729901</v>
       </c>
       <c r="O39" s="2">
-        <v>2215.9286292821798</v>
+        <v>2302.0847376249399</v>
       </c>
       <c r="Q39">
         <v>0.05</v>
@@ -2496,24 +2496,24 @@
         <v>0.05</v>
       </c>
       <c r="S39" s="2">
-        <v>1086.64912933808</v>
+        <v>1957.7940168750899</v>
       </c>
       <c r="T39" s="2">
-        <v>1973.6529760360299</v>
+        <v>2392.9295181253401</v>
       </c>
     </row>
     <row r="40" spans="2:20" x14ac:dyDescent="0.55000000000000004">
       <c r="B40">
-        <v>0.05</v>
+        <v>0.01</v>
       </c>
       <c r="C40">
-        <v>0.01</v>
+        <v>0.05</v>
       </c>
       <c r="D40" s="2">
-        <v>2066.5930147347699</v>
+        <v>2426.5791867535199</v>
       </c>
       <c r="E40" s="2">
-        <v>2067.94855553549</v>
+        <v>2426.5791867535199</v>
       </c>
       <c r="G40">
         <v>0.01</v>
@@ -2522,10 +2522,10 @@
         <v>0.05</v>
       </c>
       <c r="I40" s="2">
-        <v>1020.91946437058</v>
+        <v>1318.4902855572</v>
       </c>
       <c r="J40" s="2">
-        <v>1870.5196535792099</v>
+        <v>1353.6234044625601</v>
       </c>
       <c r="L40">
         <v>0.01</v>
@@ -2534,10 +2534,10 @@
         <v>0.05</v>
       </c>
       <c r="N40" s="2">
-        <v>2377.17172799017</v>
+        <v>2590.8584212440401</v>
       </c>
       <c r="O40" s="2">
-        <v>2396.4630338049001</v>
+        <v>2662.2536981071999</v>
       </c>
       <c r="Q40">
         <v>0.01</v>
@@ -2546,24 +2546,24 @@
         <v>0.05</v>
       </c>
       <c r="S40" s="2">
-        <v>976.04021358641205</v>
+        <v>2364.3955325111101</v>
       </c>
       <c r="T40" s="2">
-        <v>1968.0899753347801</v>
+        <v>2506.55128774884</v>
       </c>
     </row>
     <row r="41" spans="2:20" x14ac:dyDescent="0.55000000000000004">
       <c r="B41">
-        <v>0.05</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="C41">
-        <v>5.0000000000000001E-3</v>
+        <v>0.05</v>
       </c>
       <c r="D41" s="2">
-        <v>2399.0472199521701</v>
+        <v>2450.8383779280698</v>
       </c>
       <c r="E41" s="2">
-        <v>2399.0472199521701</v>
+        <v>2654.8278177269999</v>
       </c>
       <c r="G41">
         <v>5.0000000000000001E-3</v>
@@ -2572,10 +2572,10 @@
         <v>0.05</v>
       </c>
       <c r="I41" s="2">
-        <v>951.33730615075001</v>
+        <v>1874.0887874944301</v>
       </c>
       <c r="J41" s="2">
-        <v>1806.67383057038</v>
+        <v>1749.2303226496699</v>
       </c>
       <c r="L41">
         <v>5.0000000000000001E-3</v>
@@ -2584,10 +2584,10 @@
         <v>0.05</v>
       </c>
       <c r="N41" s="2">
-        <v>2087.9112678064798</v>
+        <v>2431.2232128825099</v>
       </c>
       <c r="O41" s="2">
-        <v>2167.02487257343</v>
+        <v>2447.1489721795101</v>
       </c>
       <c r="Q41">
         <v>5.0000000000000001E-3</v>
@@ -2596,24 +2596,24 @@
         <v>0.05</v>
       </c>
       <c r="S41" s="2">
-        <v>921.61311283069995</v>
+        <v>2497.72973518444</v>
       </c>
       <c r="T41" s="2">
-        <v>1873.8943850186499</v>
+        <v>2546.2391309381901</v>
       </c>
     </row>
     <row r="42" spans="2:20" x14ac:dyDescent="0.55000000000000004">
       <c r="B42">
-        <v>0.05</v>
+        <v>1E-3</v>
       </c>
       <c r="C42">
-        <v>1E-3</v>
+        <v>0.05</v>
       </c>
       <c r="D42" s="2">
-        <v>2589.12905108426</v>
+        <v>2574.40101054359</v>
       </c>
       <c r="E42" s="2">
-        <v>2654.9743425609199</v>
+        <v>2598.88577246762</v>
       </c>
       <c r="G42">
         <v>1E-3</v>
@@ -2622,10 +2622,10 @@
         <v>0.05</v>
       </c>
       <c r="I42" s="2">
-        <v>909.78829129441203</v>
+        <v>1539.32140776032</v>
       </c>
       <c r="J42" s="2">
-        <v>1757.42100670285</v>
+        <v>1527.73157131057</v>
       </c>
       <c r="L42">
         <v>1E-3</v>
@@ -2634,10 +2634,10 @@
         <v>0.05</v>
       </c>
       <c r="N42" s="2">
-        <v>2081.56863899871</v>
+        <v>2406.30157946183</v>
       </c>
       <c r="O42" s="2">
-        <v>2081.56863899871</v>
+        <v>2406.30157946183</v>
       </c>
       <c r="Q42">
         <v>1E-3</v>
@@ -2646,24 +2646,24 @@
         <v>0.05</v>
       </c>
       <c r="S42" s="2">
-        <v>918.78100114387496</v>
+        <v>2446.8462439560999</v>
       </c>
       <c r="T42" s="2">
-        <v>2080.0510999499002</v>
+        <v>2738.8302159600298</v>
       </c>
     </row>
     <row r="43" spans="2:20" x14ac:dyDescent="0.55000000000000004">
       <c r="B43">
-        <v>0.01</v>
+        <v>1</v>
       </c>
       <c r="C43">
-        <v>1</v>
+        <v>0.01</v>
       </c>
       <c r="D43" s="2">
-        <v>2156.9361378974099</v>
+        <v>0</v>
       </c>
       <c r="E43" s="2">
-        <v>2303.3454238181398</v>
+        <v>1993.51024462498</v>
       </c>
       <c r="G43">
         <v>1</v>
@@ -2672,10 +2672,10 @@
         <v>0.01</v>
       </c>
       <c r="I43" s="2">
-        <v>899.63995370340501</v>
+        <v>0</v>
       </c>
       <c r="J43" s="2">
-        <v>1761.1253733711701</v>
+        <v>1877.1696845489801</v>
       </c>
       <c r="L43">
         <v>1</v>
@@ -2684,10 +2684,10 @@
         <v>0.01</v>
       </c>
       <c r="N43" s="2">
-        <v>2210.0369415332102</v>
+        <v>0</v>
       </c>
       <c r="O43" s="2">
-        <v>2253.7482084742501</v>
+        <v>1983.76739763111</v>
       </c>
       <c r="Q43">
         <v>1</v>
@@ -2696,24 +2696,24 @@
         <v>0.01</v>
       </c>
       <c r="S43" s="2">
-        <v>1213.28961627679</v>
+        <v>0</v>
       </c>
       <c r="T43" s="2">
-        <v>2002.52214341733</v>
+        <v>2346.7248646861999</v>
       </c>
     </row>
     <row r="44" spans="2:20" x14ac:dyDescent="0.55000000000000004">
       <c r="B44">
-        <v>0.01</v>
+        <v>0.5</v>
       </c>
       <c r="C44">
-        <v>0.5</v>
+        <v>0.01</v>
       </c>
       <c r="D44" s="2">
-        <v>2205.0339109412498</v>
+        <v>0</v>
       </c>
       <c r="E44" s="2">
-        <v>2345.5867429753798</v>
+        <v>2405.63525685286</v>
       </c>
       <c r="G44">
         <v>0.5</v>
@@ -2722,10 +2722,10 @@
         <v>0.01</v>
       </c>
       <c r="I44" s="2">
-        <v>882.26565051672003</v>
+        <v>0</v>
       </c>
       <c r="J44" s="2">
-        <v>1733.27393437408</v>
+        <v>1783.5401391048199</v>
       </c>
       <c r="L44">
         <v>0.5</v>
@@ -2734,10 +2734,10 @@
         <v>0.01</v>
       </c>
       <c r="N44" s="2">
-        <v>2289.8007795225999</v>
+        <v>0</v>
       </c>
       <c r="O44" s="2">
-        <v>2455.2628243389399</v>
+        <v>1925.18000038489</v>
       </c>
       <c r="Q44">
         <v>0.5</v>
@@ -2746,24 +2746,24 @@
         <v>0.01</v>
       </c>
       <c r="S44" s="2">
-        <v>1132.89800476858</v>
+        <v>0</v>
       </c>
       <c r="T44" s="2">
-        <v>2031.61613427774</v>
+        <v>1718.1906901387299</v>
       </c>
     </row>
     <row r="45" spans="2:20" x14ac:dyDescent="0.55000000000000004">
       <c r="B45">
-        <v>0.01</v>
+        <v>0.2</v>
       </c>
       <c r="C45">
-        <v>0.2</v>
+        <v>0.01</v>
       </c>
       <c r="D45" s="2">
-        <v>2025.6617168411799</v>
+        <v>1821.60402799083</v>
       </c>
       <c r="E45" s="2">
-        <v>2217.9245269048602</v>
+        <v>1985.9863364918999</v>
       </c>
       <c r="G45">
         <v>0.2</v>
@@ -2772,10 +2772,10 @@
         <v>0.01</v>
       </c>
       <c r="I45" s="2">
-        <v>1075.5825999650899</v>
+        <v>0</v>
       </c>
       <c r="J45" s="2">
-        <v>1949.3297899096201</v>
+        <v>1993.0562067317501</v>
       </c>
       <c r="L45">
         <v>0.2</v>
@@ -2784,10 +2784,10 @@
         <v>0.01</v>
       </c>
       <c r="N45" s="2">
-        <v>1753.77141764972</v>
+        <v>1791.35003451024</v>
       </c>
       <c r="O45" s="2">
-        <v>1775.65446610189</v>
+        <v>1791.35003451024</v>
       </c>
       <c r="Q45">
         <v>0.2</v>
@@ -2796,24 +2796,24 @@
         <v>0.01</v>
       </c>
       <c r="S45" s="2">
-        <v>1014.36289948227</v>
+        <v>1116.65683161216</v>
       </c>
       <c r="T45" s="2">
-        <v>1952.68521159905</v>
+        <v>1923.85485554209</v>
       </c>
     </row>
     <row r="46" spans="2:20" x14ac:dyDescent="0.55000000000000004">
       <c r="B46">
-        <v>0.01</v>
+        <v>0.1</v>
       </c>
       <c r="C46">
-        <v>0.1</v>
+        <v>0.01</v>
       </c>
       <c r="D46" s="2">
-        <v>1907.1918937687999</v>
+        <v>1900.01997563341</v>
       </c>
       <c r="E46" s="2">
-        <v>1930.0699079671101</v>
+        <v>1900.01997563341</v>
       </c>
       <c r="G46">
         <v>0.1</v>
@@ -2822,10 +2822,10 @@
         <v>0.01</v>
       </c>
       <c r="I46" s="2">
-        <v>918.46929892946298</v>
+        <v>981.61633653682804</v>
       </c>
       <c r="J46" s="2">
-        <v>2025.4754376078899</v>
+        <v>1830.5713402099</v>
       </c>
       <c r="L46">
         <v>0.1</v>
@@ -2834,10 +2834,10 @@
         <v>0.01</v>
       </c>
       <c r="N46" s="2">
-        <v>2075.31686271323</v>
+        <v>2214.3813035462399</v>
       </c>
       <c r="O46" s="2">
-        <v>2102.5704603425202</v>
+        <v>2371.6923167180698</v>
       </c>
       <c r="Q46">
         <v>0.1</v>
@@ -2846,24 +2846,24 @@
         <v>0.01</v>
       </c>
       <c r="S46" s="2">
-        <v>1095.5967451307399</v>
+        <v>1872.2497099714501</v>
       </c>
       <c r="T46" s="2">
-        <v>1723.1647103109501</v>
+        <v>1872.2497099714501</v>
       </c>
     </row>
     <row r="47" spans="2:20" x14ac:dyDescent="0.55000000000000004">
       <c r="B47">
-        <v>0.01</v>
+        <v>0.05</v>
       </c>
       <c r="C47">
-        <v>0.05</v>
+        <v>0.01</v>
       </c>
       <c r="D47" s="2">
-        <v>2004.92863313779</v>
+        <v>2517.1092326089902</v>
       </c>
       <c r="E47" s="2">
-        <v>2127.3724464440802</v>
+        <v>2559.5318109978398</v>
       </c>
       <c r="G47">
         <v>0.05</v>
@@ -2872,10 +2872,10 @@
         <v>0.01</v>
       </c>
       <c r="I47" s="2">
-        <v>864.16071553633606</v>
+        <v>1325.1981917774599</v>
       </c>
       <c r="J47" s="2">
-        <v>1773.1349097249299</v>
+        <v>2344.79646568005</v>
       </c>
       <c r="L47">
         <v>0.05</v>
@@ -2884,10 +2884,10 @@
         <v>0.01</v>
       </c>
       <c r="N47" s="2">
-        <v>2167.7823759470498</v>
+        <v>2418.10839566601</v>
       </c>
       <c r="O47" s="2">
-        <v>2256.40625265064</v>
+        <v>2510.9650729651698</v>
       </c>
       <c r="Q47">
         <v>0.05</v>
@@ -2896,10 +2896,10 @@
         <v>0.01</v>
       </c>
       <c r="S47" s="2">
-        <v>961.39428787953295</v>
+        <v>2402.9764143371099</v>
       </c>
       <c r="T47" s="2">
-        <v>1703.8188594193</v>
+        <v>2604.1378451718301</v>
       </c>
     </row>
     <row r="48" spans="2:20" x14ac:dyDescent="0.55000000000000004">
@@ -2910,10 +2910,10 @@
         <v>0.01</v>
       </c>
       <c r="D48" s="2">
-        <v>2265.1083038142701</v>
+        <v>2547.15571983566</v>
       </c>
       <c r="E48" s="2">
-        <v>2499.7120689531498</v>
+        <v>2667.4301313532501</v>
       </c>
       <c r="G48">
         <v>0.01</v>
@@ -2922,10 +2922,10 @@
         <v>0.01</v>
       </c>
       <c r="I48" s="2">
-        <v>967.01847473458395</v>
+        <v>1529.49069501241</v>
       </c>
       <c r="J48" s="2">
-        <v>1692.6736375350099</v>
+        <v>1875.18770693076</v>
       </c>
       <c r="L48">
         <v>0.01</v>
@@ -2934,10 +2934,10 @@
         <v>0.01</v>
       </c>
       <c r="N48" s="2">
-        <v>2359.7454512437298</v>
+        <v>2539.8642308493299</v>
       </c>
       <c r="O48" s="2">
-        <v>2506.0070022425598</v>
+        <v>2705.84540262885</v>
       </c>
       <c r="Q48">
         <v>0.01</v>
@@ -2946,24 +2946,24 @@
         <v>0.01</v>
       </c>
       <c r="S48" s="2">
-        <v>592.66721710046397</v>
+        <v>2495.9334944802599</v>
       </c>
       <c r="T48" s="2">
-        <v>1970.13413457763</v>
+        <v>2669.1378593624099</v>
       </c>
     </row>
     <row r="49" spans="2:20" x14ac:dyDescent="0.55000000000000004">
       <c r="B49">
-        <v>0.01</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="C49">
-        <v>5.0000000000000001E-3</v>
+        <v>0.01</v>
       </c>
       <c r="D49" s="2">
-        <v>1840.0897058456401</v>
+        <v>2483.1424043703601</v>
       </c>
       <c r="E49" s="2">
-        <v>1845.97674991337</v>
+        <v>2490.0653798282401</v>
       </c>
       <c r="G49">
         <v>5.0000000000000001E-3</v>
@@ -2972,10 +2972,10 @@
         <v>0.01</v>
       </c>
       <c r="I49" s="2">
-        <v>1145.6863071084399</v>
+        <v>1802.92206309426</v>
       </c>
       <c r="J49" s="2">
-        <v>1608.79748139252</v>
+        <v>1825.9879930680499</v>
       </c>
       <c r="L49">
         <v>5.0000000000000001E-3</v>
@@ -2984,10 +2984,10 @@
         <v>0.01</v>
       </c>
       <c r="N49" s="2">
-        <v>2018.93400483189</v>
+        <v>2487.2670867813399</v>
       </c>
       <c r="O49" s="2">
-        <v>2019.75541641728</v>
+        <v>2613.4125892982102</v>
       </c>
       <c r="Q49">
         <v>5.0000000000000001E-3</v>
@@ -2996,24 +2996,24 @@
         <v>0.01</v>
       </c>
       <c r="S49" s="2">
-        <v>1018.50343808435</v>
+        <v>2496.8814238810901</v>
       </c>
       <c r="T49" s="2">
-        <v>1682.90250149701</v>
+        <v>2513.3595316701999</v>
       </c>
     </row>
     <row r="50" spans="2:20" x14ac:dyDescent="0.55000000000000004">
       <c r="B50">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="C50">
-        <v>1E-3</v>
+        <v>0.01</v>
       </c>
       <c r="D50" s="2">
-        <v>1950.10722057767</v>
+        <v>2479.99938115751</v>
       </c>
       <c r="E50" s="2">
-        <v>1984.28322618997</v>
+        <v>2479.99938115751</v>
       </c>
       <c r="G50">
         <v>1E-3</v>
@@ -3022,10 +3022,10 @@
         <v>0.01</v>
       </c>
       <c r="I50" s="2">
-        <v>1417.68582811023</v>
+        <v>1960.4897317110399</v>
       </c>
       <c r="J50" s="2">
-        <v>2055.5186947019602</v>
+        <v>2298.3152432443198</v>
       </c>
       <c r="L50">
         <v>1E-3</v>
@@ -3034,10 +3034,10 @@
         <v>0.01</v>
       </c>
       <c r="N50" s="2">
-        <v>2301.35831053843</v>
+        <v>2378.2729932602501</v>
       </c>
       <c r="O50" s="2">
-        <v>2507.7809626395701</v>
+        <v>2385.4307010534899</v>
       </c>
       <c r="Q50">
         <v>1E-3</v>
@@ -3046,24 +3046,24 @@
         <v>0.01</v>
       </c>
       <c r="S50" s="2">
-        <v>1203.66592212458</v>
+        <v>2483.1893985105098</v>
       </c>
       <c r="T50" s="2">
-        <v>2024.3135787777501</v>
+        <v>2647.5484227194302</v>
       </c>
     </row>
     <row r="51" spans="2:20" x14ac:dyDescent="0.55000000000000004">
       <c r="B51">
-        <v>5.0000000000000001E-3</v>
+        <v>1</v>
       </c>
       <c r="C51">
-        <v>1</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="D51" s="2">
-        <v>2234.7504106558699</v>
+        <v>0</v>
       </c>
       <c r="E51" s="2">
-        <v>2532.7113659062602</v>
+        <v>1919.6650605561599</v>
       </c>
       <c r="G51">
         <v>1</v>
@@ -3072,10 +3072,10 @@
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="I51" s="2">
-        <v>1109.0804373535</v>
+        <v>0</v>
       </c>
       <c r="J51" s="2">
-        <v>1897.8784857159999</v>
+        <v>2103.6388671044101</v>
       </c>
       <c r="L51">
         <v>1</v>
@@ -3084,10 +3084,10 @@
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="N51" s="2">
-        <v>1997.18883933558</v>
+        <v>0</v>
       </c>
       <c r="O51" s="2">
-        <v>1997.18883933558</v>
+        <v>1779.3854518575199</v>
       </c>
       <c r="Q51">
         <v>1</v>
@@ -3096,24 +3096,24 @@
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="S51" s="2">
-        <v>1147.0873432832</v>
+        <v>0</v>
       </c>
       <c r="T51" s="2">
-        <v>1848.77964524921</v>
+        <v>1931.0437097664301</v>
       </c>
     </row>
     <row r="52" spans="2:20" x14ac:dyDescent="0.55000000000000004">
       <c r="B52">
-        <v>5.0000000000000001E-3</v>
+        <v>0.5</v>
       </c>
       <c r="C52">
-        <v>0.5</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="D52" s="2">
-        <v>2360.5894343740301</v>
+        <v>0</v>
       </c>
       <c r="E52" s="2">
-        <v>2682.2810547384502</v>
+        <v>2154.8570833788299</v>
       </c>
       <c r="G52">
         <v>0.5</v>
@@ -3122,10 +3122,10 @@
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="I52" s="2">
-        <v>838.32772424753705</v>
+        <v>0</v>
       </c>
       <c r="J52" s="2">
-        <v>2021.07826402006</v>
+        <v>1636.3681244136801</v>
       </c>
       <c r="L52">
         <v>0.5</v>
@@ -3134,10 +3134,10 @@
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="N52" s="2">
-        <v>2287.81231971235</v>
+        <v>193.247074314494</v>
       </c>
       <c r="O52" s="2">
-        <v>2338.6605920953002</v>
+        <v>1923.20873162308</v>
       </c>
       <c r="Q52">
         <v>0.5</v>
@@ -3146,24 +3146,24 @@
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="S52" s="2">
-        <v>942.63347478862897</v>
+        <v>0</v>
       </c>
       <c r="T52" s="2">
-        <v>1804.4171626449299</v>
+        <v>1999.44433413661</v>
       </c>
     </row>
     <row r="53" spans="2:20" x14ac:dyDescent="0.55000000000000004">
       <c r="B53">
-        <v>5.0000000000000001E-3</v>
+        <v>0.2</v>
       </c>
       <c r="C53">
-        <v>0.2</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="D53" s="2">
-        <v>1896.5044901963599</v>
+        <v>1858.14801809248</v>
       </c>
       <c r="E53" s="2">
-        <v>1961.6001431023301</v>
+        <v>1940.6269772968101</v>
       </c>
       <c r="G53">
         <v>0.2</v>
@@ -3172,10 +3172,10 @@
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="I53" s="2">
-        <v>1066.3886871596101</v>
+        <v>0</v>
       </c>
       <c r="J53" s="2">
-        <v>2068.4986950819598</v>
+        <v>1919.2558184409299</v>
       </c>
       <c r="L53">
         <v>0.2</v>
@@ -3184,10 +3184,10 @@
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="N53" s="2">
-        <v>1995.3451689823801</v>
+        <v>2075.1117831450601</v>
       </c>
       <c r="O53" s="2">
-        <v>2066.8714575680201</v>
+        <v>2261.1911964272399</v>
       </c>
       <c r="Q53">
         <v>0.2</v>
@@ -3196,24 +3196,24 @@
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="S53" s="2">
-        <v>655.43982141572496</v>
+        <v>386.10253911731502</v>
       </c>
       <c r="T53" s="2">
-        <v>1705.3052383317499</v>
+        <v>2062.4476842225899</v>
       </c>
     </row>
     <row r="54" spans="2:20" x14ac:dyDescent="0.55000000000000004">
       <c r="B54">
-        <v>5.0000000000000001E-3</v>
+        <v>0.1</v>
       </c>
       <c r="C54">
-        <v>0.1</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="D54" s="2">
-        <v>2007.65107697288</v>
+        <v>1865.96096360039</v>
       </c>
       <c r="E54" s="2">
-        <v>2216.1871863829101</v>
+        <v>1944.3729683173101</v>
       </c>
       <c r="G54">
         <v>0.1</v>
@@ -3222,10 +3222,10 @@
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="I54" s="2">
-        <v>1162.2797909969399</v>
+        <v>980.20789151881797</v>
       </c>
       <c r="J54" s="2">
-        <v>1951.29584034039</v>
+        <v>2259.4876987138</v>
       </c>
       <c r="L54">
         <v>0.1</v>
@@ -3234,10 +3234,10 @@
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="N54" s="2">
-        <v>1907.4703383446799</v>
+        <v>2058.7618657328198</v>
       </c>
       <c r="O54" s="2">
-        <v>1938.5019758352801</v>
+        <v>2092.7749601268101</v>
       </c>
       <c r="Q54">
         <v>0.1</v>
@@ -3246,24 +3246,24 @@
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="S54" s="2">
-        <v>847.09079609840103</v>
+        <v>1652.62444642116</v>
       </c>
       <c r="T54" s="2">
-        <v>1901.3540268725401</v>
+        <v>2502.3297345730598</v>
       </c>
     </row>
     <row r="55" spans="2:20" x14ac:dyDescent="0.55000000000000004">
       <c r="B55">
-        <v>5.0000000000000001E-3</v>
+        <v>0.05</v>
       </c>
       <c r="C55">
-        <v>0.05</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="D55" s="2">
-        <v>1951.0133149456201</v>
+        <v>2590.3156840153601</v>
       </c>
       <c r="E55" s="2">
-        <v>1977.96930219721</v>
+        <v>2590.3156840153601</v>
       </c>
       <c r="G55">
         <v>0.05</v>
@@ -3272,10 +3272,10 @@
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="I55" s="2">
-        <v>969.16890804856496</v>
+        <v>1563.0684592766399</v>
       </c>
       <c r="J55" s="2">
-        <v>2038.1687922487599</v>
+        <v>2027.25916367332</v>
       </c>
       <c r="L55">
         <v>0.05</v>
@@ -3284,10 +3284,10 @@
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="N55" s="2">
-        <v>2394.9572849534802</v>
+        <v>2396.52982992754</v>
       </c>
       <c r="O55" s="2">
-        <v>2552.3358922775401</v>
+        <v>2396.52982992754</v>
       </c>
       <c r="Q55">
         <v>0.05</v>
@@ -3296,24 +3296,24 @@
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="S55" s="2">
-        <v>886.09387861247205</v>
+        <v>2412.2872344674201</v>
       </c>
       <c r="T55" s="2">
-        <v>1876.5763089193699</v>
+        <v>2458.1400459266301</v>
       </c>
     </row>
     <row r="56" spans="2:20" x14ac:dyDescent="0.55000000000000004">
       <c r="B56">
-        <v>5.0000000000000001E-3</v>
+        <v>0.01</v>
       </c>
       <c r="C56">
-        <v>0.01</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="D56" s="2">
-        <v>2182.9849278531301</v>
+        <v>2411.3138345519201</v>
       </c>
       <c r="E56" s="2">
-        <v>2182.9849278531301</v>
+        <v>2782.1569070106898</v>
       </c>
       <c r="G56">
         <v>0.01</v>
@@ -3322,10 +3322,10 @@
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="I56" s="2">
-        <v>1062.39834180304</v>
+        <v>2039.3988562585801</v>
       </c>
       <c r="J56" s="2">
-        <v>1870.5774077756701</v>
+        <v>2155.7727808760201</v>
       </c>
       <c r="L56">
         <v>0.01</v>
@@ -3334,10 +3334,10 @@
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="N56" s="2">
-        <v>2339.31584396468</v>
+        <v>2430.44360883737</v>
       </c>
       <c r="O56" s="2">
-        <v>2378.4874823743999</v>
+        <v>2504.6700761114298</v>
       </c>
       <c r="Q56">
         <v>0.01</v>
@@ -3346,10 +3346,10 @@
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="S56" s="2">
-        <v>981.54090010802702</v>
+        <v>2548.3585931759699</v>
       </c>
       <c r="T56" s="2">
-        <v>1491.2102730604399</v>
+        <v>2679.0887060207901</v>
       </c>
     </row>
     <row r="57" spans="2:20" x14ac:dyDescent="0.55000000000000004">
@@ -3360,10 +3360,10 @@
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="D57" s="2">
-        <v>1859.5493908563501</v>
+        <v>2531.7439387878999</v>
       </c>
       <c r="E57" s="2">
-        <v>1865.4587217409301</v>
+        <v>2531.7439387878999</v>
       </c>
       <c r="G57">
         <v>5.0000000000000001E-3</v>
@@ -3372,10 +3372,10 @@
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="I57" s="2">
-        <v>838.24444121224997</v>
+        <v>2154.2660988942498</v>
       </c>
       <c r="J57" s="2">
-        <v>1794.60832428713</v>
+        <v>2216.8297273716398</v>
       </c>
       <c r="L57">
         <v>5.0000000000000001E-3</v>
@@ -3384,10 +3384,10 @@
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="N57" s="2">
-        <v>2170.7335638333898</v>
+        <v>2505.2443657212398</v>
       </c>
       <c r="O57" s="2">
-        <v>2356.6330090777901</v>
+        <v>2596.6504355652701</v>
       </c>
       <c r="Q57">
         <v>5.0000000000000001E-3</v>
@@ -3396,24 +3396,24 @@
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="S57" s="2">
-        <v>803.35545193991504</v>
+        <v>2431.3440965683699</v>
       </c>
       <c r="T57" s="2">
-        <v>1897.50089985969</v>
+        <v>2648.1856473508801</v>
       </c>
     </row>
     <row r="58" spans="2:20" x14ac:dyDescent="0.55000000000000004">
       <c r="B58">
-        <v>5.0000000000000001E-3</v>
+        <v>1E-3</v>
       </c>
       <c r="C58">
-        <v>1E-3</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="D58" s="2">
-        <v>2069.9943672496902</v>
+        <v>2478.90391771961</v>
       </c>
       <c r="E58" s="2">
-        <v>2069.9943672496902</v>
+        <v>2503.29881255598</v>
       </c>
       <c r="G58">
         <v>1E-3</v>
@@ -3422,10 +3422,10 @@
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="I58" s="2">
-        <v>889.51050645833595</v>
+        <v>2389.3819941828701</v>
       </c>
       <c r="J58" s="2">
-        <v>1996.6342219587</v>
+        <v>2434.9866948551298</v>
       </c>
       <c r="L58">
         <v>1E-3</v>
@@ -3434,10 +3434,10 @@
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="N58" s="2">
-        <v>2231.3164130997002</v>
+        <v>2547.3812837523101</v>
       </c>
       <c r="O58" s="2">
-        <v>2282.9412677257401</v>
+        <v>2604.33680803174</v>
       </c>
       <c r="Q58">
         <v>1E-3</v>
@@ -3446,24 +3446,24 @@
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="S58" s="2">
-        <v>1115.1168495372399</v>
+        <v>2475.3130397745999</v>
       </c>
       <c r="T58" s="2">
-        <v>1914.77118957942</v>
+        <v>2519.6262793574301</v>
       </c>
     </row>
     <row r="59" spans="2:20" x14ac:dyDescent="0.55000000000000004">
       <c r="B59">
-        <v>1E-3</v>
+        <v>1</v>
       </c>
       <c r="C59">
-        <v>1</v>
+        <v>1E-3</v>
       </c>
       <c r="D59" s="2">
-        <v>2069.4396204914001</v>
+        <v>0</v>
       </c>
       <c r="E59" s="2">
-        <v>2233.14922041823</v>
+        <v>1893.2400629828801</v>
       </c>
       <c r="G59">
         <v>1</v>
@@ -3472,10 +3472,10 @@
         <v>1E-3</v>
       </c>
       <c r="I59" s="2">
-        <v>1040.04920413182</v>
+        <v>0</v>
       </c>
       <c r="J59" s="2">
-        <v>2089.73379491575</v>
+        <v>2289.6438287364199</v>
       </c>
       <c r="L59">
         <v>1</v>
@@ -3484,10 +3484,10 @@
         <v>1E-3</v>
       </c>
       <c r="N59" s="2">
-        <v>2350.7486966689098</v>
+        <v>0</v>
       </c>
       <c r="O59" s="2">
-        <v>2407.0874990423299</v>
+        <v>1981.4425865752401</v>
       </c>
       <c r="Q59">
         <v>1</v>
@@ -3496,24 +3496,24 @@
         <v>1E-3</v>
       </c>
       <c r="S59" s="2">
-        <v>954.01243879893798</v>
+        <v>0</v>
       </c>
       <c r="T59" s="2">
-        <v>1996.5658317228001</v>
+        <v>1935.18480801896</v>
       </c>
     </row>
     <row r="60" spans="2:20" x14ac:dyDescent="0.55000000000000004">
       <c r="B60">
-        <v>1E-3</v>
+        <v>0.5</v>
       </c>
       <c r="C60">
-        <v>0.5</v>
+        <v>1E-3</v>
       </c>
       <c r="D60" s="2">
-        <v>2287.9287761319001</v>
+        <v>0</v>
       </c>
       <c r="E60" s="2">
-        <v>2353.60144955844</v>
+        <v>1943.75385869615</v>
       </c>
       <c r="G60">
         <v>0.5</v>
@@ -3522,10 +3522,10 @@
         <v>1E-3</v>
       </c>
       <c r="I60" s="2">
-        <v>1039.6853731261001</v>
+        <v>0</v>
       </c>
       <c r="J60" s="2">
-        <v>1884.37485146942</v>
+        <v>2085.2019418045502</v>
       </c>
       <c r="L60">
         <v>0.5</v>
@@ -3534,10 +3534,10 @@
         <v>1E-3</v>
       </c>
       <c r="N60" s="2">
-        <v>2318.4848783533798</v>
+        <v>0</v>
       </c>
       <c r="O60" s="2">
-        <v>2513.7812978382599</v>
+        <v>2085.29160038283</v>
       </c>
       <c r="Q60">
         <v>0.5</v>
@@ -3546,24 +3546,24 @@
         <v>1E-3</v>
       </c>
       <c r="S60" s="2">
-        <v>826.49942580526499</v>
+        <v>0</v>
       </c>
       <c r="T60" s="2">
-        <v>1688.5913000308001</v>
+        <v>2317.03178434241</v>
       </c>
     </row>
     <row r="61" spans="2:20" x14ac:dyDescent="0.55000000000000004">
       <c r="B61">
-        <v>1E-3</v>
+        <v>0.2</v>
       </c>
       <c r="C61">
-        <v>0.2</v>
+        <v>1E-3</v>
       </c>
       <c r="D61" s="2">
-        <v>1860.7768676297701</v>
+        <v>1700.7487382289601</v>
       </c>
       <c r="E61" s="2">
-        <v>1860.7768676297701</v>
+        <v>1715.0024686074801</v>
       </c>
       <c r="G61">
         <v>0.2</v>
@@ -3572,10 +3572,10 @@
         <v>1E-3</v>
       </c>
       <c r="I61" s="2">
-        <v>1029.8649919662</v>
+        <v>0</v>
       </c>
       <c r="J61" s="2">
-        <v>1831.69979142745</v>
+        <v>1892.79982728337</v>
       </c>
       <c r="L61">
         <v>0.2</v>
@@ -3584,10 +3584,10 @@
         <v>1E-3</v>
       </c>
       <c r="N61" s="2">
-        <v>2382.5763179205801</v>
+        <v>1818.3841209505399</v>
       </c>
       <c r="O61" s="2">
-        <v>2409.6641384988202</v>
+        <v>2073.28037394577</v>
       </c>
       <c r="Q61">
         <v>0.2</v>
@@ -3596,24 +3596,24 @@
         <v>1E-3</v>
       </c>
       <c r="S61" s="2">
-        <v>1045.02854465311</v>
+        <v>567.37918053255999</v>
       </c>
       <c r="T61" s="2">
-        <v>2069.8217727830101</v>
+        <v>2417.1459542419202</v>
       </c>
     </row>
     <row r="62" spans="2:20" x14ac:dyDescent="0.55000000000000004">
       <c r="B62">
-        <v>1E-3</v>
+        <v>0.1</v>
       </c>
       <c r="C62">
-        <v>0.1</v>
+        <v>1E-3</v>
       </c>
       <c r="D62" s="2">
-        <v>2031.0703613681201</v>
+        <v>1827.7099778409399</v>
       </c>
       <c r="E62" s="2">
-        <v>2483.6955215651301</v>
+        <v>1864.3924110160301</v>
       </c>
       <c r="G62">
         <v>0.1</v>
@@ -3622,10 +3622,10 @@
         <v>1E-3</v>
       </c>
       <c r="I62" s="2">
-        <v>1172.7963224149401</v>
+        <v>1228.84952347428</v>
       </c>
       <c r="J62" s="2">
-        <v>1783.46086614656</v>
+        <v>2029.51531386027</v>
       </c>
       <c r="L62">
         <v>0.1</v>
@@ -3634,10 +3634,10 @@
         <v>1E-3</v>
       </c>
       <c r="N62" s="2">
-        <v>2083.3508100274198</v>
+        <v>1868.70750603696</v>
       </c>
       <c r="O62" s="2">
-        <v>2197.4935614077099</v>
+        <v>1905.5992067888999</v>
       </c>
       <c r="Q62">
         <v>0.1</v>
@@ -3646,24 +3646,24 @@
         <v>1E-3</v>
       </c>
       <c r="S62" s="2">
-        <v>622.30805758970905</v>
+        <v>2103.0465344622999</v>
       </c>
       <c r="T62" s="2">
-        <v>1675.7648275321901</v>
+        <v>2495.5717504409599</v>
       </c>
     </row>
     <row r="63" spans="2:20" x14ac:dyDescent="0.55000000000000004">
       <c r="B63">
-        <v>1E-3</v>
+        <v>0.05</v>
       </c>
       <c r="C63">
-        <v>0.05</v>
+        <v>1E-3</v>
       </c>
       <c r="D63" s="2">
-        <v>2189.5786428894398</v>
+        <v>2412.3587307364401</v>
       </c>
       <c r="E63" s="2">
-        <v>2376.8031371458501</v>
+        <v>2485.38192009457</v>
       </c>
       <c r="G63">
         <v>0.05</v>
@@ -3672,10 +3672,10 @@
         <v>1E-3</v>
       </c>
       <c r="I63" s="2">
-        <v>824.35931525787805</v>
+        <v>1471.43748901461</v>
       </c>
       <c r="J63" s="2">
-        <v>2004.41086234465</v>
+        <v>2273.9126222974101</v>
       </c>
       <c r="L63">
         <v>0.05</v>
@@ -3684,10 +3684,10 @@
         <v>1E-3</v>
       </c>
       <c r="N63" s="2">
-        <v>2072.56439850271</v>
+        <v>2434.9047380579</v>
       </c>
       <c r="O63" s="2">
-        <v>2090.2274956606698</v>
+        <v>2529.9313504681199</v>
       </c>
       <c r="Q63">
         <v>0.05</v>
@@ -3696,24 +3696,24 @@
         <v>1E-3</v>
       </c>
       <c r="S63" s="2">
-        <v>1142.9512279815399</v>
+        <v>2514.7593442370899</v>
       </c>
       <c r="T63" s="2">
-        <v>1842.7404848292899</v>
+        <v>2514.7593442370799</v>
       </c>
     </row>
     <row r="64" spans="2:20" x14ac:dyDescent="0.55000000000000004">
       <c r="B64">
-        <v>1E-3</v>
+        <v>0.01</v>
       </c>
       <c r="C64">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="D64" s="2">
-        <v>1804.3879555394301</v>
+        <v>2622.82846303211</v>
       </c>
       <c r="E64" s="2">
-        <v>1853.6839573058701</v>
+        <v>2751.9941571978202</v>
       </c>
       <c r="G64">
         <v>0.01</v>
@@ -3722,10 +3722,10 @@
         <v>1E-3</v>
       </c>
       <c r="I64" s="2">
-        <v>930.97125464243402</v>
+        <v>2105.97684259168</v>
       </c>
       <c r="J64" s="2">
-        <v>1762.7250007729399</v>
+        <v>2265.2017225128898</v>
       </c>
       <c r="L64">
         <v>0.01</v>
@@ -3734,10 +3734,10 @@
         <v>1E-3</v>
       </c>
       <c r="N64" s="2">
-        <v>2176.44822979426</v>
+        <v>2494.5515318275602</v>
       </c>
       <c r="O64" s="2">
-        <v>2242.1578833958501</v>
+        <v>2753.0349257090302</v>
       </c>
       <c r="Q64">
         <v>0.01</v>
@@ -3746,24 +3746,24 @@
         <v>1E-3</v>
       </c>
       <c r="S64" s="2">
-        <v>1414.7389019793</v>
+        <v>2511.2253200526402</v>
       </c>
       <c r="T64" s="2">
-        <v>1711.65916568886</v>
+        <v>2511.2253200526402</v>
       </c>
     </row>
     <row r="65" spans="2:20" x14ac:dyDescent="0.55000000000000004">
       <c r="B65">
-        <v>1E-3</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="C65">
-        <v>5.0000000000000001E-3</v>
+        <v>1E-3</v>
       </c>
       <c r="D65" s="2">
-        <v>2114.3379784557601</v>
+        <v>2483.4029508369599</v>
       </c>
       <c r="E65" s="2">
-        <v>2298.2795868611402</v>
+        <v>2568.1474107124</v>
       </c>
       <c r="G65">
         <v>5.0000000000000001E-3</v>
@@ -3772,10 +3772,10 @@
         <v>1E-3</v>
       </c>
       <c r="I65" s="2">
-        <v>1200.0618631929899</v>
+        <v>2358.6798560239899</v>
       </c>
       <c r="J65" s="2">
-        <v>2170.9267654782898</v>
+        <v>2582.7527752598799</v>
       </c>
       <c r="L65">
         <v>5.0000000000000001E-3</v>
@@ -3784,10 +3784,10 @@
         <v>1E-3</v>
       </c>
       <c r="N65" s="2">
-        <v>2232.4886629020102</v>
+        <v>2569.41926856586</v>
       </c>
       <c r="O65" s="2">
-        <v>2275.9159146788402</v>
+        <v>2589.9086803400301</v>
       </c>
       <c r="Q65">
         <v>5.0000000000000001E-3</v>
@@ -3796,10 +3796,10 @@
         <v>1E-3</v>
       </c>
       <c r="S65" s="2">
-        <v>880.60042432910996</v>
+        <v>2491.7820616858598</v>
       </c>
       <c r="T65" s="2">
-        <v>1652.3808727369601</v>
+        <v>2491.7820616858598</v>
       </c>
     </row>
     <row r="66" spans="2:20" x14ac:dyDescent="0.55000000000000004">
@@ -3810,10 +3810,10 @@
         <v>1E-3</v>
       </c>
       <c r="D66" s="2">
-        <v>2158.3702687912901</v>
+        <v>2541.49455242766</v>
       </c>
       <c r="E66" s="2">
-        <v>2284.2455338725899</v>
+        <v>2627.7001780129699</v>
       </c>
       <c r="G66">
         <v>1E-3</v>
@@ -3822,10 +3822,10 @@
         <v>1E-3</v>
       </c>
       <c r="I66" s="2">
-        <v>1116.9816127279601</v>
+        <v>1841.11050181922</v>
       </c>
       <c r="J66" s="2">
-        <v>2098.0115162677398</v>
+        <v>2059.1903159256199</v>
       </c>
       <c r="L66">
         <v>1E-3</v>
@@ -3834,10 +3834,10 @@
         <v>1E-3</v>
       </c>
       <c r="N66" s="2">
-        <v>1993.48516498699</v>
+        <v>2493.49902497417</v>
       </c>
       <c r="O66" s="2">
-        <v>2141.2432231538401</v>
+        <v>2830.7592225796998</v>
       </c>
       <c r="Q66">
         <v>1E-3</v>
@@ -3846,10 +3846,10 @@
         <v>1E-3</v>
       </c>
       <c r="S66" s="2">
-        <v>786.44670202762097</v>
+        <v>2410.6559538524298</v>
       </c>
       <c r="T66" s="2">
-        <v>1802.5190171151501</v>
+        <v>2424.44512385396</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
same samples for each experiment and more results
</commit_message>
<xml_diff>
--- a/results/result_summary_epsilon_support.xlsx
+++ b/results/result_summary_epsilon_support.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Robert\Documents\_Work\Research\00_Workshop\data_valuation\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EED0A275-21CC-40B5-A05B-78C03940762D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AB9A0AF-F018-4100-9445-E4957D953E99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" activeTab="1" xr2:uid="{FFE2B131-66A4-4E63-8C13-A75AF38B9E2B}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="23">
   <si>
     <t>lam2</t>
   </si>
@@ -106,6 +106,9 @@
   </si>
   <si>
     <t>Each experiment is sampled and run 10 times and the results averaged to reduce the impact of individual sample outcomes</t>
+  </si>
+  <si>
+    <t>Each experiment is performed with the same set of 10 samples</t>
   </si>
 </sst>
 </file>
@@ -475,10 +478,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{056EC552-3B33-4C7A-BFE0-F85E370CBE75}">
-  <dimension ref="B2:C11"/>
+  <dimension ref="B2:C12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -561,6 +564,11 @@
         <v>21</v>
       </c>
     </row>
+    <row r="12" spans="2:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="C12" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -570,21 +578,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BB6718F-3B8A-4B8D-842A-7EE6474384A0}">
   <dimension ref="B1:T66"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="U11" sqref="U11"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData>
     <row r="1" spans="2:20" x14ac:dyDescent="0.55000000000000004">
       <c r="B1" s="4" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C1" s="4"/>
       <c r="D1" s="4"/>
       <c r="E1" s="4"/>
       <c r="G1" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H1" s="4"/>
       <c r="I1" s="4"/>
@@ -760,7 +768,7 @@
         <v>1</v>
       </c>
       <c r="D5" s="2">
-        <v>1774.7211885793499</v>
+        <v>0</v>
       </c>
       <c r="E5" s="2">
         <v>0</v>
@@ -772,7 +780,7 @@
         <v>1</v>
       </c>
       <c r="I5" s="2">
-        <v>0</v>
+        <v>1864.97502115713</v>
       </c>
       <c r="J5" s="2">
         <v>0</v>
@@ -784,7 +792,7 @@
         <v>1</v>
       </c>
       <c r="N5" s="2">
-        <v>1855.95921197143</v>
+        <v>1867.4204205589199</v>
       </c>
       <c r="O5" s="2">
         <v>0</v>
@@ -796,7 +804,7 @@
         <v>1</v>
       </c>
       <c r="S5" s="2">
-        <v>1025.9709953481699</v>
+        <v>766.55476474970305</v>
       </c>
       <c r="T5" s="2">
         <v>0</v>
@@ -810,7 +818,7 @@
         <v>1</v>
       </c>
       <c r="D6" s="2">
-        <v>1821.5228289618899</v>
+        <v>923.13094567902203</v>
       </c>
       <c r="E6" s="2">
         <v>0</v>
@@ -822,7 +830,7 @@
         <v>1</v>
       </c>
       <c r="I6" s="2">
-        <v>862.84691356399605</v>
+        <v>1949.5355928832701</v>
       </c>
       <c r="J6" s="2">
         <v>0</v>
@@ -834,7 +842,7 @@
         <v>1</v>
       </c>
       <c r="N6" s="2">
-        <v>1818.4728810709901</v>
+        <v>1923.3704140589</v>
       </c>
       <c r="O6" s="2">
         <v>0</v>
@@ -846,7 +854,7 @@
         <v>1</v>
       </c>
       <c r="S6" s="2">
-        <v>1921.5473837582599</v>
+        <v>1460.6488161187101</v>
       </c>
       <c r="T6" s="2">
         <v>0</v>
@@ -860,7 +868,7 @@
         <v>1</v>
       </c>
       <c r="D7" s="2">
-        <v>1971.8544722638401</v>
+        <v>1474.1642262949699</v>
       </c>
       <c r="E7" s="2">
         <v>0</v>
@@ -872,7 +880,7 @@
         <v>1</v>
       </c>
       <c r="I7" s="2">
-        <v>1564.99392789282</v>
+        <v>2009.8284306922901</v>
       </c>
       <c r="J7" s="2">
         <v>0</v>
@@ -884,7 +892,7 @@
         <v>1</v>
       </c>
       <c r="N7" s="2">
-        <v>1755.1086326319601</v>
+        <v>1983.6632518679301</v>
       </c>
       <c r="O7" s="2">
         <v>0</v>
@@ -896,7 +904,7 @@
         <v>1</v>
       </c>
       <c r="S7" s="2">
-        <v>2064.8039404741498</v>
+        <v>2009.8284306922901</v>
       </c>
       <c r="T7" s="2">
         <v>0</v>
@@ -910,7 +918,7 @@
         <v>1</v>
       </c>
       <c r="D8" s="2">
-        <v>1807.1907572103</v>
+        <v>2009.8284306922901</v>
       </c>
       <c r="E8" s="2">
         <v>0</v>
@@ -922,7 +930,7 @@
         <v>1</v>
       </c>
       <c r="I8" s="2">
-        <v>1453.29138596096</v>
+        <v>2009.8284306922901</v>
       </c>
       <c r="J8" s="2">
         <v>0</v>
@@ -934,7 +942,7 @@
         <v>1</v>
       </c>
       <c r="N8" s="2">
-        <v>2078.8307401534998</v>
+        <v>1983.6632518679301</v>
       </c>
       <c r="O8" s="2">
         <v>0</v>
@@ -946,7 +954,7 @@
         <v>1</v>
       </c>
       <c r="S8" s="2">
-        <v>2008.30155007959</v>
+        <v>2009.8284306922901</v>
       </c>
       <c r="T8" s="2">
         <v>0</v>
@@ -960,7 +968,7 @@
         <v>1</v>
       </c>
       <c r="D9" s="2">
-        <v>2261.2066057606698</v>
+        <v>2009.8284306922901</v>
       </c>
       <c r="E9" s="2">
         <v>0</v>
@@ -972,7 +980,7 @@
         <v>1</v>
       </c>
       <c r="I9" s="2">
-        <v>1817.2135735827901</v>
+        <v>2009.8284306922901</v>
       </c>
       <c r="J9" s="2">
         <v>0</v>
@@ -984,7 +992,7 @@
         <v>1</v>
       </c>
       <c r="N9" s="2">
-        <v>1822.7283052140699</v>
+        <v>1983.6632518679301</v>
       </c>
       <c r="O9" s="2">
         <v>0</v>
@@ -996,7 +1004,7 @@
         <v>1</v>
       </c>
       <c r="S9" s="2">
-        <v>1901.9968061663101</v>
+        <v>2009.8284306922901</v>
       </c>
       <c r="T9" s="2">
         <v>0</v>
@@ -1010,7 +1018,7 @@
         <v>1</v>
       </c>
       <c r="D10" s="2">
-        <v>1688.10070322158</v>
+        <v>2009.8284306922901</v>
       </c>
       <c r="E10" s="2">
         <v>0</v>
@@ -1022,7 +1030,7 @@
         <v>1</v>
       </c>
       <c r="I10" s="2">
-        <v>1734.21819535281</v>
+        <v>2009.8284306922901</v>
       </c>
       <c r="J10" s="2">
         <v>0</v>
@@ -1034,7 +1042,7 @@
         <v>1</v>
       </c>
       <c r="N10" s="2">
-        <v>1776.4662402389299</v>
+        <v>1983.6632518679301</v>
       </c>
       <c r="O10" s="2">
         <v>0</v>
@@ -1046,7 +1054,7 @@
         <v>1</v>
       </c>
       <c r="S10" s="2">
-        <v>1970.7990690317599</v>
+        <v>2009.8284306922901</v>
       </c>
       <c r="T10" s="2">
         <v>0</v>
@@ -1087,7 +1095,7 @@
         <v>0</v>
       </c>
       <c r="O11" s="2">
-        <v>1842.1837407123501</v>
+        <v>2265.5057535810101</v>
       </c>
       <c r="Q11">
         <v>1</v>
@@ -1099,7 +1107,7 @@
         <v>0</v>
       </c>
       <c r="T11" s="2">
-        <v>202.68990830557399</v>
+        <v>677.19045619096505</v>
       </c>
     </row>
     <row r="12" spans="2:20" x14ac:dyDescent="0.55000000000000004">
@@ -1137,7 +1145,7 @@
         <v>0</v>
       </c>
       <c r="O12" s="2">
-        <v>2389.0100540627</v>
+        <v>2265.5057535810101</v>
       </c>
       <c r="Q12">
         <v>0.5</v>
@@ -1149,7 +1157,7 @@
         <v>0</v>
       </c>
       <c r="T12" s="2">
-        <v>275.45246069986302</v>
+        <v>677.19045619096505</v>
       </c>
     </row>
     <row r="13" spans="2:20" x14ac:dyDescent="0.55000000000000004">
@@ -1160,7 +1168,7 @@
         <v>0.5</v>
       </c>
       <c r="D13" s="2">
-        <v>1754.7658721038499</v>
+        <v>0</v>
       </c>
       <c r="E13" s="2">
         <v>0</v>
@@ -1172,7 +1180,7 @@
         <v>0.5</v>
       </c>
       <c r="I13" s="2">
-        <v>0</v>
+        <v>1864.97502115713</v>
       </c>
       <c r="J13" s="2">
         <v>0</v>
@@ -1184,10 +1192,10 @@
         <v>0.5</v>
       </c>
       <c r="N13" s="2">
-        <v>1811.7985341313099</v>
+        <v>1867.4204205589199</v>
       </c>
       <c r="O13" s="2">
-        <v>1913.2414332052799</v>
+        <v>2265.5057535810101</v>
       </c>
       <c r="Q13">
         <v>0.2</v>
@@ -1196,10 +1204,10 @@
         <v>0.5</v>
       </c>
       <c r="S13" s="2">
-        <v>315.01279961052398</v>
+        <v>766.55476474970305</v>
       </c>
       <c r="T13" s="2">
-        <v>0</v>
+        <v>677.19045619096505</v>
       </c>
     </row>
     <row r="14" spans="2:20" x14ac:dyDescent="0.55000000000000004">
@@ -1210,7 +1218,7 @@
         <v>0.5</v>
       </c>
       <c r="D14" s="2">
-        <v>2069.0995554153401</v>
+        <v>923.13094567902203</v>
       </c>
       <c r="E14" s="2">
         <v>0</v>
@@ -1222,7 +1230,7 @@
         <v>0.5</v>
       </c>
       <c r="I14" s="2">
-        <v>1522.9394689417099</v>
+        <v>1949.5355928832701</v>
       </c>
       <c r="J14" s="2">
         <v>0</v>
@@ -1234,10 +1242,10 @@
         <v>0.5</v>
       </c>
       <c r="N14" s="2">
-        <v>1838.27704805554</v>
+        <v>1923.3704140589</v>
       </c>
       <c r="O14" s="2">
-        <v>2108.4744578311702</v>
+        <v>2265.8343705183902</v>
       </c>
       <c r="Q14">
         <v>0.1</v>
@@ -1246,10 +1254,10 @@
         <v>0.5</v>
       </c>
       <c r="S14" s="2">
-        <v>1843.25010776832</v>
+        <v>1460.6488161187101</v>
       </c>
       <c r="T14" s="2">
-        <v>351.50907054785802</v>
+        <v>677.51907312833805</v>
       </c>
     </row>
     <row r="15" spans="2:20" x14ac:dyDescent="0.55000000000000004">
@@ -1260,7 +1268,7 @@
         <v>0.5</v>
       </c>
       <c r="D15" s="2">
-        <v>1884.6993504223101</v>
+        <v>1474.1642262949699</v>
       </c>
       <c r="E15" s="2">
         <v>0</v>
@@ -1272,7 +1280,7 @@
         <v>0.5</v>
       </c>
       <c r="I15" s="2">
-        <v>1182.4490826804699</v>
+        <v>2009.8284306922901</v>
       </c>
       <c r="J15" s="2">
         <v>0</v>
@@ -1284,10 +1292,10 @@
         <v>0.5</v>
       </c>
       <c r="N15" s="2">
-        <v>1960.2884586913699</v>
+        <v>2009.8284306922901</v>
       </c>
       <c r="O15" s="2">
-        <v>2105.73101402672</v>
+        <v>2284.7340523345802</v>
       </c>
       <c r="Q15">
         <v>0.05</v>
@@ -1296,10 +1304,10 @@
         <v>0.5</v>
       </c>
       <c r="S15" s="2">
-        <v>1697.7489510385501</v>
+        <v>2009.8284306922901</v>
       </c>
       <c r="T15" s="2">
-        <v>0</v>
+        <v>677.51907312833805</v>
       </c>
     </row>
     <row r="16" spans="2:20" x14ac:dyDescent="0.55000000000000004">
@@ -1310,7 +1318,7 @@
         <v>0.5</v>
       </c>
       <c r="D16" s="2">
-        <v>1803.9006853012099</v>
+        <v>2009.8284306922901</v>
       </c>
       <c r="E16" s="2">
         <v>0</v>
@@ -1322,7 +1330,7 @@
         <v>0.5</v>
       </c>
       <c r="I16" s="2">
-        <v>1471.34559899233</v>
+        <v>2009.8284306922901</v>
       </c>
       <c r="J16" s="2">
         <v>0</v>
@@ -1334,10 +1342,10 @@
         <v>0.5</v>
       </c>
       <c r="N16" s="2">
-        <v>2277.5007157047899</v>
+        <v>2009.8284306922901</v>
       </c>
       <c r="O16" s="2">
-        <v>2453.0452245246001</v>
+        <v>2284.7340523345702</v>
       </c>
       <c r="Q16">
         <v>0.01</v>
@@ -1346,10 +1354,10 @@
         <v>0.5</v>
       </c>
       <c r="S16" s="2">
-        <v>1846.1282347772999</v>
+        <v>2009.8284306922901</v>
       </c>
       <c r="T16" s="2">
-        <v>318.04394476259603</v>
+        <v>677.51907312833805</v>
       </c>
     </row>
     <row r="17" spans="2:20" x14ac:dyDescent="0.55000000000000004">
@@ -1360,7 +1368,7 @@
         <v>0.5</v>
       </c>
       <c r="D17" s="2">
-        <v>2078.4308952393999</v>
+        <v>2009.8284306922901</v>
       </c>
       <c r="E17" s="2">
         <v>0</v>
@@ -1372,7 +1380,7 @@
         <v>0.5</v>
       </c>
       <c r="I17" s="2">
-        <v>2014.16878099766</v>
+        <v>2009.8284306922901</v>
       </c>
       <c r="J17" s="2">
         <v>0</v>
@@ -1384,10 +1392,10 @@
         <v>0.5</v>
       </c>
       <c r="N17" s="2">
-        <v>1755.4324084508601</v>
+        <v>2009.8284306922901</v>
       </c>
       <c r="O17" s="2">
-        <v>1764.3266476768599</v>
+        <v>2284.7340523345702</v>
       </c>
       <c r="Q17">
         <v>5.0000000000000001E-3</v>
@@ -1396,10 +1404,10 @@
         <v>0.5</v>
       </c>
       <c r="S17" s="2">
-        <v>1984.6118347813799</v>
+        <v>2009.8284306922901</v>
       </c>
       <c r="T17" s="2">
-        <v>289.84990194267601</v>
+        <v>677.51907312833805</v>
       </c>
     </row>
     <row r="18" spans="2:20" x14ac:dyDescent="0.55000000000000004">
@@ -1410,7 +1418,7 @@
         <v>0.5</v>
       </c>
       <c r="D18" s="2">
-        <v>1947.79583328688</v>
+        <v>2009.8284306922901</v>
       </c>
       <c r="E18" s="2">
         <v>0</v>
@@ -1422,7 +1430,7 @@
         <v>0.5</v>
       </c>
       <c r="I18" s="2">
-        <v>1824.8040391910699</v>
+        <v>2009.8284306922901</v>
       </c>
       <c r="J18" s="2">
         <v>0</v>
@@ -1434,10 +1442,10 @@
         <v>0.5</v>
       </c>
       <c r="N18" s="2">
-        <v>1890.4135154628</v>
+        <v>2009.8284306922901</v>
       </c>
       <c r="O18" s="2">
-        <v>1890.4135154628</v>
+        <v>2284.7340523345702</v>
       </c>
       <c r="Q18">
         <v>1E-3</v>
@@ -1446,10 +1454,10 @@
         <v>0.5</v>
       </c>
       <c r="S18" s="2">
-        <v>1985.7994219360701</v>
+        <v>2009.8284306922901</v>
       </c>
       <c r="T18" s="2">
-        <v>0</v>
+        <v>677.51907312833805</v>
       </c>
     </row>
     <row r="19" spans="2:20" x14ac:dyDescent="0.55000000000000004">
@@ -1463,7 +1471,7 @@
         <v>0</v>
       </c>
       <c r="E19" s="2">
-        <v>1989.74432766731</v>
+        <v>240.80233939600799</v>
       </c>
       <c r="G19">
         <v>1</v>
@@ -1475,7 +1483,7 @@
         <v>0</v>
       </c>
       <c r="J19" s="2">
-        <v>78.940582530916998</v>
+        <v>2284.4054353972001</v>
       </c>
       <c r="L19">
         <v>1</v>
@@ -1487,7 +1495,7 @@
         <v>0</v>
       </c>
       <c r="O19" s="2">
-        <v>1863.42895523164</v>
+        <v>2265.5057535810101</v>
       </c>
       <c r="Q19">
         <v>1</v>
@@ -1499,7 +1507,7 @@
         <v>0</v>
       </c>
       <c r="T19" s="2">
-        <v>2129.4688885268502</v>
+        <v>2284.4054353972001</v>
       </c>
     </row>
     <row r="20" spans="2:20" x14ac:dyDescent="0.55000000000000004">
@@ -1513,7 +1521,7 @@
         <v>0</v>
       </c>
       <c r="E20" s="2">
-        <v>1859.1061274364399</v>
+        <v>240.80233939600799</v>
       </c>
       <c r="G20">
         <v>0.5</v>
@@ -1525,7 +1533,7 @@
         <v>0</v>
       </c>
       <c r="J20" s="2">
-        <v>74.706935248917603</v>
+        <v>2284.4054353972001</v>
       </c>
       <c r="L20">
         <v>0.5</v>
@@ -1534,10 +1542,10 @@
         <v>0.2</v>
       </c>
       <c r="N20" s="2">
-        <v>0</v>
+        <v>161.24562421063001</v>
       </c>
       <c r="O20" s="2">
-        <v>2146.7841141004201</v>
+        <v>2265.5057535810101</v>
       </c>
       <c r="Q20">
         <v>0.5</v>
@@ -1549,7 +1557,7 @@
         <v>0</v>
       </c>
       <c r="T20" s="2">
-        <v>1792.8239776448099</v>
+        <v>2284.4054353972001</v>
       </c>
     </row>
     <row r="21" spans="2:20" x14ac:dyDescent="0.55000000000000004">
@@ -1560,10 +1568,10 @@
         <v>0.2</v>
       </c>
       <c r="D21" s="2">
-        <v>1924.9650934061899</v>
+        <v>0</v>
       </c>
       <c r="E21" s="2">
-        <v>2227.33316670967</v>
+        <v>240.80233939600799</v>
       </c>
       <c r="G21">
         <v>0.2</v>
@@ -1572,10 +1580,10 @@
         <v>0.2</v>
       </c>
       <c r="I21" s="2">
-        <v>0</v>
+        <v>1891.1401999815</v>
       </c>
       <c r="J21" s="2">
-        <v>181.58841206989999</v>
+        <v>2284.4054353972001</v>
       </c>
       <c r="L21">
         <v>0.2</v>
@@ -1584,10 +1592,10 @@
         <v>0.2</v>
       </c>
       <c r="N21" s="2">
-        <v>1925.75205768208</v>
+        <v>1893.5855993832899</v>
       </c>
       <c r="O21" s="2">
-        <v>1973.49250467395</v>
+        <v>2284.4054353972001</v>
       </c>
       <c r="Q21">
         <v>0.2</v>
@@ -1596,10 +1604,10 @@
         <v>0.2</v>
       </c>
       <c r="S21" s="2">
-        <v>511.02676429606203</v>
+        <v>792.71994357406697</v>
       </c>
       <c r="T21" s="2">
-        <v>1906.5130300138101</v>
+        <v>2284.4054353972001</v>
       </c>
     </row>
     <row r="22" spans="2:20" x14ac:dyDescent="0.55000000000000004">
@@ -1610,10 +1618,10 @@
         <v>0.2</v>
       </c>
       <c r="D22" s="2">
-        <v>1758.80166741938</v>
+        <v>923.13094567902203</v>
       </c>
       <c r="E22" s="2">
-        <v>1760.1843009337899</v>
+        <v>240.80233939600799</v>
       </c>
       <c r="G22">
         <v>0.1</v>
@@ -1622,10 +1630,10 @@
         <v>0.2</v>
       </c>
       <c r="I22" s="2">
-        <v>1056.36308724843</v>
+        <v>1949.5355928832701</v>
       </c>
       <c r="J22" s="2">
-        <v>0</v>
+        <v>2284.7340523345802</v>
       </c>
       <c r="L22">
         <v>0.1</v>
@@ -1634,10 +1642,10 @@
         <v>0.2</v>
       </c>
       <c r="N22" s="2">
-        <v>1829.5809639776101</v>
+        <v>1949.5355928832701</v>
       </c>
       <c r="O22" s="2">
-        <v>1959.40348035289</v>
+        <v>2284.7340523345702</v>
       </c>
       <c r="Q22">
         <v>0.1</v>
@@ -1646,10 +1654,10 @@
         <v>0.2</v>
       </c>
       <c r="S22" s="2">
-        <v>1884.73372163414</v>
+        <v>1460.6488161187101</v>
       </c>
       <c r="T22" s="2">
-        <v>1814.65781693587</v>
+        <v>2284.7340523345702</v>
       </c>
     </row>
     <row r="23" spans="2:20" x14ac:dyDescent="0.55000000000000004">
@@ -1660,10 +1668,10 @@
         <v>0.2</v>
       </c>
       <c r="D23" s="2">
-        <v>2218.0890359125701</v>
+        <v>1474.1642262949699</v>
       </c>
       <c r="E23" s="2">
-        <v>2167.7160830233802</v>
+        <v>240.94164330228801</v>
       </c>
       <c r="G23">
         <v>0.05</v>
@@ -1672,10 +1680,10 @@
         <v>0.2</v>
       </c>
       <c r="I23" s="2">
-        <v>1216.74189715069</v>
+        <v>2009.8284306922901</v>
       </c>
       <c r="J23" s="2">
-        <v>97.020740175976698</v>
+        <v>2284.7340523345802</v>
       </c>
       <c r="L23">
         <v>0.05</v>
@@ -1684,10 +1692,10 @@
         <v>0.2</v>
       </c>
       <c r="N23" s="2">
-        <v>2064.7836159450098</v>
+        <v>2009.8284306922901</v>
       </c>
       <c r="O23" s="2">
-        <v>2214.6345593076999</v>
+        <v>2284.7340523345702</v>
       </c>
       <c r="Q23">
         <v>0.05</v>
@@ -1696,10 +1704,10 @@
         <v>0.2</v>
       </c>
       <c r="S23" s="2">
-        <v>1796.8365529488799</v>
+        <v>2009.8284306922901</v>
       </c>
       <c r="T23" s="2">
-        <v>1796.8365529488799</v>
+        <v>2284.7340523345702</v>
       </c>
     </row>
     <row r="24" spans="2:20" x14ac:dyDescent="0.55000000000000004">
@@ -1710,10 +1718,10 @@
         <v>0.2</v>
       </c>
       <c r="D24" s="2">
-        <v>2099.36068740583</v>
+        <v>2009.8284306922901</v>
       </c>
       <c r="E24" s="2">
-        <v>2217.8936413760298</v>
+        <v>240.94164330228801</v>
       </c>
       <c r="G24">
         <v>0.01</v>
@@ -1722,10 +1730,10 @@
         <v>0.2</v>
       </c>
       <c r="I24" s="2">
-        <v>1541.5299843483101</v>
+        <v>2009.8284306922901</v>
       </c>
       <c r="J24" s="2">
-        <v>181.66549237631</v>
+        <v>2284.7340523345702</v>
       </c>
       <c r="L24">
         <v>0.01</v>
@@ -1734,10 +1742,10 @@
         <v>0.2</v>
       </c>
       <c r="N24" s="2">
-        <v>1810.7760254062</v>
+        <v>2009.8284306922901</v>
       </c>
       <c r="O24" s="2">
-        <v>1975.1918096536899</v>
+        <v>2284.7340523345702</v>
       </c>
       <c r="Q24">
         <v>0.01</v>
@@ -1746,10 +1754,10 @@
         <v>0.2</v>
       </c>
       <c r="S24" s="2">
-        <v>1989.4310200575001</v>
+        <v>2009.8284306922901</v>
       </c>
       <c r="T24" s="2">
-        <v>1982.5861194822601</v>
+        <v>2284.7340523345702</v>
       </c>
     </row>
     <row r="25" spans="2:20" x14ac:dyDescent="0.55000000000000004">
@@ -1760,10 +1768,10 @@
         <v>0.2</v>
       </c>
       <c r="D25" s="2">
-        <v>1785.16344472487</v>
+        <v>2009.8284306922901</v>
       </c>
       <c r="E25" s="2">
-        <v>1799.79440028149</v>
+        <v>240.94164330228801</v>
       </c>
       <c r="G25">
         <v>5.0000000000000001E-3</v>
@@ -1772,10 +1780,10 @@
         <v>0.2</v>
       </c>
       <c r="I25" s="2">
-        <v>1575.3778339155799</v>
+        <v>2009.8284306922901</v>
       </c>
       <c r="J25" s="2">
-        <v>189.538338226501</v>
+        <v>2284.7340523345702</v>
       </c>
       <c r="L25">
         <v>5.0000000000000001E-3</v>
@@ -1784,10 +1792,10 @@
         <v>0.2</v>
       </c>
       <c r="N25" s="2">
-        <v>1922.4415137475501</v>
+        <v>2009.8284306922901</v>
       </c>
       <c r="O25" s="2">
-        <v>1942.04043048482</v>
+        <v>2284.7340523345702</v>
       </c>
       <c r="Q25">
         <v>5.0000000000000001E-3</v>
@@ -1796,10 +1804,10 @@
         <v>0.2</v>
       </c>
       <c r="S25" s="2">
-        <v>1676.56624130153</v>
+        <v>2009.8284306922901</v>
       </c>
       <c r="T25" s="2">
-        <v>1526.56624130153</v>
+        <v>2284.7340523345702</v>
       </c>
     </row>
     <row r="26" spans="2:20" x14ac:dyDescent="0.55000000000000004">
@@ -1810,10 +1818,10 @@
         <v>0.2</v>
       </c>
       <c r="D26" s="2">
-        <v>1854.2794190597299</v>
+        <v>2009.8284306922901</v>
       </c>
       <c r="E26" s="2">
-        <v>1886.90048592121</v>
+        <v>240.94164330228801</v>
       </c>
       <c r="G26">
         <v>1E-3</v>
@@ -1822,10 +1830,10 @@
         <v>0.2</v>
       </c>
       <c r="I26" s="2">
-        <v>1884.8263364289201</v>
+        <v>2009.8284306922901</v>
       </c>
       <c r="J26" s="2">
-        <v>87.974306547856003</v>
+        <v>2284.7340523345802</v>
       </c>
       <c r="L26">
         <v>1E-3</v>
@@ -1834,10 +1842,10 @@
         <v>0.2</v>
       </c>
       <c r="N26" s="2">
-        <v>1657.5146567230199</v>
+        <v>2009.8284306922901</v>
       </c>
       <c r="O26" s="2">
-        <v>1670.8090382099101</v>
+        <v>2284.7340523345702</v>
       </c>
       <c r="Q26">
         <v>1E-3</v>
@@ -1846,10 +1854,10 @@
         <v>0.2</v>
       </c>
       <c r="S26" s="2">
-        <v>2077.4484728849902</v>
+        <v>2009.8284306922901</v>
       </c>
       <c r="T26" s="2">
-        <v>2081.1881192739902</v>
+        <v>2284.7340523345802</v>
       </c>
     </row>
     <row r="27" spans="2:20" x14ac:dyDescent="0.55000000000000004">
@@ -1863,7 +1871,7 @@
         <v>0</v>
       </c>
       <c r="E27" s="2">
-        <v>2173.62085634508</v>
+        <v>1299.07861753323</v>
       </c>
       <c r="G27">
         <v>1</v>
@@ -1875,7 +1883,7 @@
         <v>0</v>
       </c>
       <c r="J27" s="2">
-        <v>1020.00958427921</v>
+        <v>2284.4054353972001</v>
       </c>
       <c r="L27">
         <v>1</v>
@@ -1887,7 +1895,7 @@
         <v>0</v>
       </c>
       <c r="O27" s="2">
-        <v>2011.5008555511499</v>
+        <v>2265.5057535810101</v>
       </c>
       <c r="Q27">
         <v>1</v>
@@ -1899,7 +1907,7 @@
         <v>0</v>
       </c>
       <c r="T27" s="2">
-        <v>1832.0108045371301</v>
+        <v>2284.4054353972001</v>
       </c>
     </row>
     <row r="28" spans="2:20" x14ac:dyDescent="0.55000000000000004">
@@ -1913,7 +1921,7 @@
         <v>0</v>
       </c>
       <c r="E28" s="2">
-        <v>2100.4894370673501</v>
+        <v>1299.07861753323</v>
       </c>
       <c r="G28">
         <v>0.5</v>
@@ -1925,7 +1933,7 @@
         <v>0</v>
       </c>
       <c r="J28" s="2">
-        <v>1103.21083315429</v>
+        <v>2284.4054353972001</v>
       </c>
       <c r="L28">
         <v>0.5</v>
@@ -1937,7 +1945,7 @@
         <v>0</v>
       </c>
       <c r="O28" s="2">
-        <v>1978.29924534918</v>
+        <v>2265.5057535810101</v>
       </c>
       <c r="Q28">
         <v>0.5</v>
@@ -1949,7 +1957,7 @@
         <v>0</v>
       </c>
       <c r="T28" s="2">
-        <v>1831.0159791410999</v>
+        <v>2284.4054353972001</v>
       </c>
     </row>
     <row r="29" spans="2:20" x14ac:dyDescent="0.55000000000000004">
@@ -1960,10 +1968,10 @@
         <v>0.1</v>
       </c>
       <c r="D29" s="2">
-        <v>1812.6562676012099</v>
+        <v>0</v>
       </c>
       <c r="E29" s="2">
-        <v>1915.7515387702099</v>
+        <v>1299.07861753323</v>
       </c>
       <c r="G29">
         <v>0.2</v>
@@ -1972,10 +1980,10 @@
         <v>0.1</v>
       </c>
       <c r="I29" s="2">
-        <v>0</v>
+        <v>1891.1401999815</v>
       </c>
       <c r="J29" s="2">
-        <v>1244.12671434053</v>
+        <v>2284.4054353972001</v>
       </c>
       <c r="L29">
         <v>0.2</v>
@@ -1984,10 +1992,10 @@
         <v>0.1</v>
       </c>
       <c r="N29" s="2">
-        <v>1784.8432802781899</v>
+        <v>1893.5855993832899</v>
       </c>
       <c r="O29" s="2">
-        <v>1816.1643213999801</v>
+        <v>2284.4054353972001</v>
       </c>
       <c r="Q29">
         <v>0.2</v>
@@ -1996,10 +2004,10 @@
         <v>0.1</v>
       </c>
       <c r="S29" s="2">
-        <v>319.33837661331103</v>
+        <v>792.71994357406697</v>
       </c>
       <c r="T29" s="2">
-        <v>1698.3548042151299</v>
+        <v>2284.4054353972001</v>
       </c>
     </row>
     <row r="30" spans="2:20" x14ac:dyDescent="0.55000000000000004">
@@ -2010,10 +2018,10 @@
         <v>0.1</v>
       </c>
       <c r="D30" s="2">
-        <v>1767.6496223245099</v>
+        <v>923.13094567902203</v>
       </c>
       <c r="E30" s="2">
-        <v>1987.5659211889199</v>
+        <v>1299.07861753323</v>
       </c>
       <c r="G30">
         <v>0.1</v>
@@ -2022,10 +2030,10 @@
         <v>0.1</v>
       </c>
       <c r="I30" s="2">
-        <v>742.03833221343598</v>
+        <v>1949.5355928832701</v>
       </c>
       <c r="J30" s="2">
-        <v>1048.81763916523</v>
+        <v>2284.7340523345702</v>
       </c>
       <c r="L30">
         <v>0.1</v>
@@ -2034,10 +2042,10 @@
         <v>0.1</v>
       </c>
       <c r="N30" s="2">
-        <v>2001.4539636503</v>
+        <v>1949.5355928832701</v>
       </c>
       <c r="O30" s="2">
-        <v>2100.6236837947099</v>
+        <v>2284.7340523345702</v>
       </c>
       <c r="Q30">
         <v>0.1</v>
@@ -2046,10 +2054,10 @@
         <v>0.1</v>
       </c>
       <c r="S30" s="2">
-        <v>1644.0003433473601</v>
+        <v>1460.6488161187101</v>
       </c>
       <c r="T30" s="2">
-        <v>2329.951916431</v>
+        <v>2284.7340523345702</v>
       </c>
     </row>
     <row r="31" spans="2:20" x14ac:dyDescent="0.55000000000000004">
@@ -2060,10 +2068,10 @@
         <v>0.1</v>
       </c>
       <c r="D31" s="2">
-        <v>1809.81556069369</v>
+        <v>1474.1642262949699</v>
       </c>
       <c r="E31" s="2">
-        <v>1993.6980278579899</v>
+        <v>1299.26001438242</v>
       </c>
       <c r="G31">
         <v>0.05</v>
@@ -2072,10 +2080,10 @@
         <v>0.1</v>
       </c>
       <c r="I31" s="2">
-        <v>1109.2361095373301</v>
+        <v>2009.8284306922901</v>
       </c>
       <c r="J31" s="2">
-        <v>1137.9263820035101</v>
+        <v>2284.7340523345702</v>
       </c>
       <c r="L31">
         <v>0.05</v>
@@ -2084,10 +2092,10 @@
         <v>0.1</v>
       </c>
       <c r="N31" s="2">
-        <v>2309.1486254121301</v>
+        <v>2009.8284306922901</v>
       </c>
       <c r="O31" s="2">
-        <v>2484.5990547111001</v>
+        <v>2284.7340523345702</v>
       </c>
       <c r="Q31">
         <v>0.05</v>
@@ -2096,10 +2104,10 @@
         <v>0.1</v>
       </c>
       <c r="S31" s="2">
-        <v>1885.2642723132101</v>
+        <v>2009.8284306922901</v>
       </c>
       <c r="T31" s="2">
-        <v>1986.05608711541</v>
+        <v>2284.7340523345702</v>
       </c>
     </row>
     <row r="32" spans="2:20" x14ac:dyDescent="0.55000000000000004">
@@ -2110,10 +2118,10 @@
         <v>0.1</v>
       </c>
       <c r="D32" s="2">
-        <v>2261.3286243838702</v>
+        <v>2009.8284306922901</v>
       </c>
       <c r="E32" s="2">
-        <v>2280.9290700085098</v>
+        <v>1299.26001438242</v>
       </c>
       <c r="G32">
         <v>0.01</v>
@@ -2122,10 +2130,10 @@
         <v>0.1</v>
       </c>
       <c r="I32" s="2">
-        <v>1665.7725536871601</v>
+        <v>2009.8284306922901</v>
       </c>
       <c r="J32" s="2">
-        <v>1040.9882914396801</v>
+        <v>2284.7340523345702</v>
       </c>
       <c r="L32">
         <v>0.01</v>
@@ -2134,10 +2142,10 @@
         <v>0.1</v>
       </c>
       <c r="N32" s="2">
-        <v>2020.1316297298999</v>
+        <v>2009.8284306922901</v>
       </c>
       <c r="O32" s="2">
-        <v>2202.4566164124799</v>
+        <v>2284.7340523345702</v>
       </c>
       <c r="Q32">
         <v>0.01</v>
@@ -2146,10 +2154,10 @@
         <v>0.1</v>
       </c>
       <c r="S32" s="2">
-        <v>2320.0197192097098</v>
+        <v>2009.8284306922901</v>
       </c>
       <c r="T32" s="2">
-        <v>2375.2665253492601</v>
+        <v>2284.7340523345802</v>
       </c>
     </row>
     <row r="33" spans="2:20" x14ac:dyDescent="0.55000000000000004">
@@ -2160,10 +2168,10 @@
         <v>0.1</v>
       </c>
       <c r="D33" s="2">
-        <v>2342.88820511833</v>
+        <v>2009.8284306922901</v>
       </c>
       <c r="E33" s="2">
-        <v>2377.4111757328001</v>
+        <v>1299.26001438242</v>
       </c>
       <c r="G33">
         <v>5.0000000000000001E-3</v>
@@ -2172,10 +2180,10 @@
         <v>0.1</v>
       </c>
       <c r="I33" s="2">
-        <v>1743.10750650367</v>
+        <v>2009.8284306922901</v>
       </c>
       <c r="J33" s="2">
-        <v>993.33389263768299</v>
+        <v>2284.7340523345702</v>
       </c>
       <c r="L33">
         <v>5.0000000000000001E-3</v>
@@ -2184,10 +2192,10 @@
         <v>0.1</v>
       </c>
       <c r="N33" s="2">
-        <v>2269.3672373146801</v>
+        <v>2009.8284306922901</v>
       </c>
       <c r="O33" s="2">
-        <v>2440.26373061512</v>
+        <v>2284.7340523345702</v>
       </c>
       <c r="Q33">
         <v>5.0000000000000001E-3</v>
@@ -2196,10 +2204,10 @@
         <v>0.1</v>
       </c>
       <c r="S33" s="2">
-        <v>2251.01435479462</v>
+        <v>2009.8284306922901</v>
       </c>
       <c r="T33" s="2">
-        <v>2266.0175200609901</v>
+        <v>2284.7340523345802</v>
       </c>
     </row>
     <row r="34" spans="2:20" x14ac:dyDescent="0.55000000000000004">
@@ -2210,10 +2218,10 @@
         <v>0.1</v>
       </c>
       <c r="D34" s="2">
-        <v>1765.6645407718399</v>
+        <v>2009.8284306922901</v>
       </c>
       <c r="E34" s="2">
-        <v>1765.6645407718399</v>
+        <v>1299.26001438242</v>
       </c>
       <c r="G34">
         <v>1E-3</v>
@@ -2222,10 +2230,10 @@
         <v>0.1</v>
       </c>
       <c r="I34" s="2">
-        <v>1709.2400087045901</v>
+        <v>2076.76135945226</v>
       </c>
       <c r="J34" s="2">
-        <v>1085.4164449559501</v>
+        <v>2351.66698109454</v>
       </c>
       <c r="L34">
         <v>1E-3</v>
@@ -2234,10 +2242,10 @@
         <v>0.1</v>
       </c>
       <c r="N34" s="2">
-        <v>2421.2476065720698</v>
+        <v>2076.76135945226</v>
       </c>
       <c r="O34" s="2">
-        <v>2421.2476065720698</v>
+        <v>2351.66698109454</v>
       </c>
       <c r="Q34">
         <v>1E-3</v>
@@ -2246,10 +2254,10 @@
         <v>0.1</v>
       </c>
       <c r="S34" s="2">
-        <v>2191.53083925792</v>
+        <v>2076.76135945226</v>
       </c>
       <c r="T34" s="2">
-        <v>2253.5894235983001</v>
+        <v>2351.66698109454</v>
       </c>
     </row>
     <row r="35" spans="2:20" x14ac:dyDescent="0.55000000000000004">
@@ -2263,7 +2271,7 @@
         <v>0</v>
       </c>
       <c r="E35" s="2">
-        <v>2044.8160381898099</v>
+        <v>1554.9594179046901</v>
       </c>
       <c r="G35">
         <v>1</v>
@@ -2275,7 +2283,7 @@
         <v>0</v>
       </c>
       <c r="J35" s="2">
-        <v>1546.13362517002</v>
+        <v>2284.4054353972001</v>
       </c>
       <c r="L35">
         <v>1</v>
@@ -2287,7 +2295,7 @@
         <v>0</v>
       </c>
       <c r="O35" s="2">
-        <v>1982.83346763947</v>
+        <v>2265.5057535810101</v>
       </c>
       <c r="Q35">
         <v>1</v>
@@ -2299,7 +2307,7 @@
         <v>0</v>
       </c>
       <c r="T35" s="2">
-        <v>2159.2894443679002</v>
+        <v>2284.4054353972001</v>
       </c>
     </row>
     <row r="36" spans="2:20" x14ac:dyDescent="0.55000000000000004">
@@ -2313,7 +2321,7 @@
         <v>0</v>
       </c>
       <c r="E36" s="2">
-        <v>2138.3434793424499</v>
+        <v>1554.9594179046901</v>
       </c>
       <c r="G36">
         <v>0.5</v>
@@ -2325,7 +2333,7 @@
         <v>0</v>
       </c>
       <c r="J36" s="2">
-        <v>1628.3925784861499</v>
+        <v>2284.4054353972001</v>
       </c>
       <c r="L36">
         <v>0.5</v>
@@ -2337,7 +2345,7 @@
         <v>0</v>
       </c>
       <c r="O36" s="2">
-        <v>1797.0283366384899</v>
+        <v>2265.5057535810101</v>
       </c>
       <c r="Q36">
         <v>0.5</v>
@@ -2349,7 +2357,7 @@
         <v>0</v>
       </c>
       <c r="T36" s="2">
-        <v>1914.6136565582699</v>
+        <v>2284.4054353972001</v>
       </c>
     </row>
     <row r="37" spans="2:20" x14ac:dyDescent="0.55000000000000004">
@@ -2360,10 +2368,10 @@
         <v>0.05</v>
       </c>
       <c r="D37" s="2">
-        <v>1972.8589930103001</v>
+        <v>0</v>
       </c>
       <c r="E37" s="2">
-        <v>2663.6412610039301</v>
+        <v>1554.9594179046901</v>
       </c>
       <c r="G37">
         <v>0.2</v>
@@ -2372,10 +2380,10 @@
         <v>0.05</v>
       </c>
       <c r="I37" s="2">
-        <v>0</v>
+        <v>1891.1401999815</v>
       </c>
       <c r="J37" s="2">
-        <v>1591.07025581321</v>
+        <v>2284.4054353972001</v>
       </c>
       <c r="L37">
         <v>0.2</v>
@@ -2384,10 +2392,10 @@
         <v>0.05</v>
       </c>
       <c r="N37" s="2">
-        <v>1753.52855094595</v>
+        <v>1893.5855993832899</v>
       </c>
       <c r="O37" s="2">
-        <v>1807.2902710029</v>
+        <v>2284.4054353972001</v>
       </c>
       <c r="Q37">
         <v>0.2</v>
@@ -2396,10 +2404,10 @@
         <v>0.05</v>
       </c>
       <c r="S37" s="2">
-        <v>397.39163017096803</v>
+        <v>792.71994357406697</v>
       </c>
       <c r="T37" s="2">
-        <v>2091.3718594359898</v>
+        <v>2284.4054353972001</v>
       </c>
     </row>
     <row r="38" spans="2:20" x14ac:dyDescent="0.55000000000000004">
@@ -2410,10 +2418,10 @@
         <v>0.05</v>
       </c>
       <c r="D38" s="2">
-        <v>1898.99931462677</v>
+        <v>923.13094567902203</v>
       </c>
       <c r="E38" s="2">
-        <v>1921.2313015448201</v>
+        <v>1554.9594179046901</v>
       </c>
       <c r="G38">
         <v>0.1</v>
@@ -2422,10 +2430,10 @@
         <v>0.05</v>
       </c>
       <c r="I38" s="2">
-        <v>1107.92819107891</v>
+        <v>1949.5355928832701</v>
       </c>
       <c r="J38" s="2">
-        <v>1604.62492588856</v>
+        <v>2284.7340523345702</v>
       </c>
       <c r="L38">
         <v>0.1</v>
@@ -2434,10 +2442,10 @@
         <v>0.05</v>
       </c>
       <c r="N38" s="2">
-        <v>1839.16771971658</v>
+        <v>1949.5355928832701</v>
       </c>
       <c r="O38" s="2">
-        <v>1930.68926354316</v>
+        <v>2284.7340523345702</v>
       </c>
       <c r="Q38">
         <v>0.1</v>
@@ -2446,10 +2454,10 @@
         <v>0.05</v>
       </c>
       <c r="S38" s="2">
-        <v>1975.8760601292299</v>
+        <v>1460.6488161187101</v>
       </c>
       <c r="T38" s="2">
-        <v>2273.74109216537</v>
+        <v>2284.7340523345702</v>
       </c>
     </row>
     <row r="39" spans="2:20" x14ac:dyDescent="0.55000000000000004">
@@ -2460,10 +2468,10 @@
         <v>0.05</v>
       </c>
       <c r="D39" s="2">
-        <v>2284.9296869434502</v>
+        <v>1474.1642262949699</v>
       </c>
       <c r="E39" s="2">
-        <v>2437.4869179915199</v>
+        <v>1555.1719109124599</v>
       </c>
       <c r="G39">
         <v>0.05</v>
@@ -2472,10 +2480,10 @@
         <v>0.05</v>
       </c>
       <c r="I39" s="2">
-        <v>1234.3194776755799</v>
+        <v>2076.76135945226</v>
       </c>
       <c r="J39" s="2">
-        <v>2000.7752249391999</v>
+        <v>2351.66698109454</v>
       </c>
       <c r="L39">
         <v>0.05</v>
@@ -2484,10 +2492,10 @@
         <v>0.05</v>
       </c>
       <c r="N39" s="2">
-        <v>2277.4795221729901</v>
+        <v>2076.76135945226</v>
       </c>
       <c r="O39" s="2">
-        <v>2302.0847376249399</v>
+        <v>2351.66698109454</v>
       </c>
       <c r="Q39">
         <v>0.05</v>
@@ -2496,10 +2504,10 @@
         <v>0.05</v>
       </c>
       <c r="S39" s="2">
-        <v>1957.7940168750899</v>
+        <v>2076.76135945226</v>
       </c>
       <c r="T39" s="2">
-        <v>2392.9295181253401</v>
+        <v>2351.66698109454</v>
       </c>
     </row>
     <row r="40" spans="2:20" x14ac:dyDescent="0.55000000000000004">
@@ -2510,10 +2518,10 @@
         <v>0.05</v>
       </c>
       <c r="D40" s="2">
-        <v>2426.5791867535199</v>
+        <v>2009.8284306922901</v>
       </c>
       <c r="E40" s="2">
-        <v>2426.5791867535199</v>
+        <v>1555.1719109124599</v>
       </c>
       <c r="G40">
         <v>0.01</v>
@@ -2522,10 +2530,10 @@
         <v>0.05</v>
       </c>
       <c r="I40" s="2">
-        <v>1318.4902855572</v>
+        <v>2352.0263018611199</v>
       </c>
       <c r="J40" s="2">
-        <v>1353.6234044625601</v>
+        <v>2626.9319235034</v>
       </c>
       <c r="L40">
         <v>0.01</v>
@@ -2534,10 +2542,10 @@
         <v>0.05</v>
       </c>
       <c r="N40" s="2">
-        <v>2590.8584212440401</v>
+        <v>2352.0263018611199</v>
       </c>
       <c r="O40" s="2">
-        <v>2662.2536981071999</v>
+        <v>2626.9319235034</v>
       </c>
       <c r="Q40">
         <v>0.01</v>
@@ -2546,10 +2554,10 @@
         <v>0.05</v>
       </c>
       <c r="S40" s="2">
-        <v>2364.3955325111101</v>
+        <v>2352.0263018611199</v>
       </c>
       <c r="T40" s="2">
-        <v>2506.55128774884</v>
+        <v>2626.9319235034</v>
       </c>
     </row>
     <row r="41" spans="2:20" x14ac:dyDescent="0.55000000000000004">
@@ -2560,10 +2568,10 @@
         <v>0.05</v>
       </c>
       <c r="D41" s="2">
-        <v>2450.8383779280698</v>
+        <v>2009.8284306922901</v>
       </c>
       <c r="E41" s="2">
-        <v>2654.8278177269999</v>
+        <v>1555.1719109124599</v>
       </c>
       <c r="G41">
         <v>5.0000000000000001E-3</v>
@@ -2572,10 +2580,10 @@
         <v>0.05</v>
       </c>
       <c r="I41" s="2">
-        <v>1874.0887874944301</v>
+        <v>2352.0263018611199</v>
       </c>
       <c r="J41" s="2">
-        <v>1749.2303226496699</v>
+        <v>2626.9319235034</v>
       </c>
       <c r="L41">
         <v>5.0000000000000001E-3</v>
@@ -2584,10 +2592,10 @@
         <v>0.05</v>
       </c>
       <c r="N41" s="2">
-        <v>2431.2232128825099</v>
+        <v>2352.0263018611199</v>
       </c>
       <c r="O41" s="2">
-        <v>2447.1489721795101</v>
+        <v>2626.9319235034</v>
       </c>
       <c r="Q41">
         <v>5.0000000000000001E-3</v>
@@ -2596,10 +2604,10 @@
         <v>0.05</v>
       </c>
       <c r="S41" s="2">
-        <v>2497.72973518444</v>
+        <v>2352.0263018611199</v>
       </c>
       <c r="T41" s="2">
-        <v>2546.2391309381901</v>
+        <v>2626.9319235034</v>
       </c>
     </row>
     <row r="42" spans="2:20" x14ac:dyDescent="0.55000000000000004">
@@ -2610,10 +2618,10 @@
         <v>0.05</v>
       </c>
       <c r="D42" s="2">
-        <v>2574.40101054359</v>
+        <v>2009.8284306922901</v>
       </c>
       <c r="E42" s="2">
-        <v>2598.88577246762</v>
+        <v>1555.1719109124599</v>
       </c>
       <c r="G42">
         <v>1E-3</v>
@@ -2622,10 +2630,10 @@
         <v>0.05</v>
       </c>
       <c r="I42" s="2">
-        <v>1539.32140776032</v>
+        <v>2352.0263018611199</v>
       </c>
       <c r="J42" s="2">
-        <v>1527.73157131057</v>
+        <v>2626.9319235034</v>
       </c>
       <c r="L42">
         <v>1E-3</v>
@@ -2634,10 +2642,10 @@
         <v>0.05</v>
       </c>
       <c r="N42" s="2">
-        <v>2406.30157946183</v>
+        <v>2352.0263018611199</v>
       </c>
       <c r="O42" s="2">
-        <v>2406.30157946183</v>
+        <v>2626.9319235034</v>
       </c>
       <c r="Q42">
         <v>1E-3</v>
@@ -2646,10 +2654,10 @@
         <v>0.05</v>
       </c>
       <c r="S42" s="2">
-        <v>2446.8462439560999</v>
+        <v>2352.0263018611199</v>
       </c>
       <c r="T42" s="2">
-        <v>2738.8302159600298</v>
+        <v>2626.9319235034</v>
       </c>
     </row>
     <row r="43" spans="2:20" x14ac:dyDescent="0.55000000000000004">
@@ -2663,7 +2671,7 @@
         <v>0</v>
       </c>
       <c r="E43" s="2">
-        <v>1993.51024462498</v>
+        <v>1919.9502963862899</v>
       </c>
       <c r="G43">
         <v>1</v>
@@ -2675,7 +2683,7 @@
         <v>0</v>
       </c>
       <c r="J43" s="2">
-        <v>1877.1696845489801</v>
+        <v>2284.4054353972001</v>
       </c>
       <c r="L43">
         <v>1</v>
@@ -2687,7 +2695,7 @@
         <v>0</v>
       </c>
       <c r="O43" s="2">
-        <v>1983.76739763111</v>
+        <v>2265.5057535810101</v>
       </c>
       <c r="Q43">
         <v>1</v>
@@ -2699,7 +2707,7 @@
         <v>0</v>
       </c>
       <c r="T43" s="2">
-        <v>2346.7248646861999</v>
+        <v>2284.4054353972001</v>
       </c>
     </row>
     <row r="44" spans="2:20" x14ac:dyDescent="0.55000000000000004">
@@ -2713,7 +2721,7 @@
         <v>0</v>
       </c>
       <c r="E44" s="2">
-        <v>2405.63525685286</v>
+        <v>1919.9502963862899</v>
       </c>
       <c r="G44">
         <v>0.5</v>
@@ -2725,7 +2733,7 @@
         <v>0</v>
       </c>
       <c r="J44" s="2">
-        <v>1783.5401391048199</v>
+        <v>2284.4054353972001</v>
       </c>
       <c r="L44">
         <v>0.5</v>
@@ -2734,10 +2742,10 @@
         <v>0.01</v>
       </c>
       <c r="N44" s="2">
-        <v>0</v>
+        <v>537.76846457254499</v>
       </c>
       <c r="O44" s="2">
-        <v>1925.18000038489</v>
+        <v>2265.5057535810101</v>
       </c>
       <c r="Q44">
         <v>0.5</v>
@@ -2749,7 +2757,7 @@
         <v>0</v>
       </c>
       <c r="T44" s="2">
-        <v>1718.1906901387299</v>
+        <v>2284.4054353972001</v>
       </c>
     </row>
     <row r="45" spans="2:20" x14ac:dyDescent="0.55000000000000004">
@@ -2760,10 +2768,10 @@
         <v>0.01</v>
       </c>
       <c r="D45" s="2">
-        <v>1821.60402799083</v>
+        <v>0</v>
       </c>
       <c r="E45" s="2">
-        <v>1985.9863364918999</v>
+        <v>1919.9502963862899</v>
       </c>
       <c r="G45">
         <v>0.2</v>
@@ -2772,10 +2780,10 @@
         <v>0.01</v>
       </c>
       <c r="I45" s="2">
-        <v>0</v>
+        <v>1891.1401999815</v>
       </c>
       <c r="J45" s="2">
-        <v>1993.0562067317501</v>
+        <v>2284.4054353972001</v>
       </c>
       <c r="L45">
         <v>0.2</v>
@@ -2784,10 +2792,10 @@
         <v>0.01</v>
       </c>
       <c r="N45" s="2">
-        <v>1791.35003451024</v>
+        <v>1893.5855993832899</v>
       </c>
       <c r="O45" s="2">
-        <v>1791.35003451024</v>
+        <v>2284.4054353972001</v>
       </c>
       <c r="Q45">
         <v>0.2</v>
@@ -2796,10 +2804,10 @@
         <v>0.01</v>
       </c>
       <c r="S45" s="2">
-        <v>1116.65683161216</v>
+        <v>792.71994357406697</v>
       </c>
       <c r="T45" s="2">
-        <v>1923.85485554209</v>
+        <v>2284.4054353972001</v>
       </c>
     </row>
     <row r="46" spans="2:20" x14ac:dyDescent="0.55000000000000004">
@@ -2810,10 +2818,10 @@
         <v>0.01</v>
       </c>
       <c r="D46" s="2">
-        <v>1900.01997563341</v>
+        <v>923.13094567902203</v>
       </c>
       <c r="E46" s="2">
-        <v>1900.01997563341</v>
+        <v>1919.9502963862899</v>
       </c>
       <c r="G46">
         <v>0.1</v>
@@ -2822,10 +2830,10 @@
         <v>0.01</v>
       </c>
       <c r="I46" s="2">
-        <v>981.61633653682804</v>
+        <v>1949.5355928832701</v>
       </c>
       <c r="J46" s="2">
-        <v>1830.5713402099</v>
+        <v>2284.7340523345802</v>
       </c>
       <c r="L46">
         <v>0.1</v>
@@ -2834,10 +2842,10 @@
         <v>0.01</v>
       </c>
       <c r="N46" s="2">
-        <v>2214.3813035462399</v>
+        <v>1949.5355928832701</v>
       </c>
       <c r="O46" s="2">
-        <v>2371.6923167180698</v>
+        <v>2284.7340523345702</v>
       </c>
       <c r="Q46">
         <v>0.1</v>
@@ -2846,10 +2854,10 @@
         <v>0.01</v>
       </c>
       <c r="S46" s="2">
-        <v>1872.2497099714501</v>
+        <v>1460.6488161187101</v>
       </c>
       <c r="T46" s="2">
-        <v>1872.2497099714501</v>
+        <v>2284.7340523345702</v>
       </c>
     </row>
     <row r="47" spans="2:20" x14ac:dyDescent="0.55000000000000004">
@@ -2860,10 +2868,10 @@
         <v>0.01</v>
       </c>
       <c r="D47" s="2">
-        <v>2517.1092326089902</v>
+        <v>1474.1642262949699</v>
       </c>
       <c r="E47" s="2">
-        <v>2559.5318109978398</v>
+        <v>1920.2789133236699</v>
       </c>
       <c r="G47">
         <v>0.05</v>
@@ -2872,10 +2880,10 @@
         <v>0.01</v>
       </c>
       <c r="I47" s="2">
-        <v>1325.1981917774599</v>
+        <v>2352.0263018611199</v>
       </c>
       <c r="J47" s="2">
-        <v>2344.79646568005</v>
+        <v>2626.9319235034</v>
       </c>
       <c r="L47">
         <v>0.05</v>
@@ -2884,10 +2892,10 @@
         <v>0.01</v>
       </c>
       <c r="N47" s="2">
-        <v>2418.10839566601</v>
+        <v>2352.0263018611199</v>
       </c>
       <c r="O47" s="2">
-        <v>2510.9650729651698</v>
+        <v>2626.9319235034</v>
       </c>
       <c r="Q47">
         <v>0.05</v>
@@ -2896,10 +2904,10 @@
         <v>0.01</v>
       </c>
       <c r="S47" s="2">
-        <v>2402.9764143371099</v>
+        <v>2352.0263018611199</v>
       </c>
       <c r="T47" s="2">
-        <v>2604.1378451718301</v>
+        <v>2626.9319235034</v>
       </c>
     </row>
     <row r="48" spans="2:20" x14ac:dyDescent="0.55000000000000004">
@@ -2910,10 +2918,10 @@
         <v>0.01</v>
       </c>
       <c r="D48" s="2">
-        <v>2547.15571983566</v>
+        <v>2009.8284306922901</v>
       </c>
       <c r="E48" s="2">
-        <v>2667.4301313532501</v>
+        <v>1920.2789133236699</v>
       </c>
       <c r="G48">
         <v>0.01</v>
@@ -2922,10 +2930,10 @@
         <v>0.01</v>
       </c>
       <c r="I48" s="2">
-        <v>1529.49069501241</v>
+        <v>2420.82272903186</v>
       </c>
       <c r="J48" s="2">
-        <v>1875.18770693076</v>
+        <v>2695.7283506741401</v>
       </c>
       <c r="L48">
         <v>0.01</v>
@@ -2934,10 +2942,10 @@
         <v>0.01</v>
       </c>
       <c r="N48" s="2">
-        <v>2539.8642308493299</v>
+        <v>2420.82272903186</v>
       </c>
       <c r="O48" s="2">
-        <v>2705.84540262885</v>
+        <v>2695.7283506741401</v>
       </c>
       <c r="Q48">
         <v>0.01</v>
@@ -2946,10 +2954,10 @@
         <v>0.01</v>
       </c>
       <c r="S48" s="2">
-        <v>2495.9334944802599</v>
+        <v>2420.82272903186</v>
       </c>
       <c r="T48" s="2">
-        <v>2669.1378593624099</v>
+        <v>2695.7283506741401</v>
       </c>
     </row>
     <row r="49" spans="2:20" x14ac:dyDescent="0.55000000000000004">
@@ -2960,10 +2968,10 @@
         <v>0.01</v>
       </c>
       <c r="D49" s="2">
-        <v>2483.1424043703601</v>
+        <v>2061.1072920461202</v>
       </c>
       <c r="E49" s="2">
-        <v>2490.0653798282401</v>
+        <v>1971.5577746775</v>
       </c>
       <c r="G49">
         <v>5.0000000000000001E-3</v>
@@ -2972,10 +2980,10 @@
         <v>0.01</v>
       </c>
       <c r="I49" s="2">
-        <v>1802.92206309426</v>
+        <v>2472.1015903856901</v>
       </c>
       <c r="J49" s="2">
-        <v>1825.9879930680499</v>
+        <v>2747.0072120279801</v>
       </c>
       <c r="L49">
         <v>5.0000000000000001E-3</v>
@@ -2984,10 +2992,10 @@
         <v>0.01</v>
       </c>
       <c r="N49" s="2">
-        <v>2487.2670867813399</v>
+        <v>2472.1015903856901</v>
       </c>
       <c r="O49" s="2">
-        <v>2613.4125892982102</v>
+        <v>2747.0072120279801</v>
       </c>
       <c r="Q49">
         <v>5.0000000000000001E-3</v>
@@ -2996,10 +3004,10 @@
         <v>0.01</v>
       </c>
       <c r="S49" s="2">
-        <v>2496.8814238810901</v>
+        <v>2472.1015903856901</v>
       </c>
       <c r="T49" s="2">
-        <v>2513.3595316701999</v>
+        <v>2747.0072120279801</v>
       </c>
     </row>
     <row r="50" spans="2:20" x14ac:dyDescent="0.55000000000000004">
@@ -3010,10 +3018,10 @@
         <v>0.01</v>
       </c>
       <c r="D50" s="2">
-        <v>2479.99938115751</v>
+        <v>2061.1072920461202</v>
       </c>
       <c r="E50" s="2">
-        <v>2479.99938115751</v>
+        <v>1971.5577746775</v>
       </c>
       <c r="G50">
         <v>1E-3</v>
@@ -3022,10 +3030,10 @@
         <v>0.01</v>
       </c>
       <c r="I50" s="2">
-        <v>1960.4897317110399</v>
+        <v>2472.1015903856901</v>
       </c>
       <c r="J50" s="2">
-        <v>2298.3152432443198</v>
+        <v>2747.0072120279801</v>
       </c>
       <c r="L50">
         <v>1E-3</v>
@@ -3034,10 +3042,10 @@
         <v>0.01</v>
       </c>
       <c r="N50" s="2">
-        <v>2378.2729932602501</v>
+        <v>2472.1015903856901</v>
       </c>
       <c r="O50" s="2">
-        <v>2385.4307010534899</v>
+        <v>2747.0072120279801</v>
       </c>
       <c r="Q50">
         <v>1E-3</v>
@@ -3046,10 +3054,10 @@
         <v>0.01</v>
       </c>
       <c r="S50" s="2">
-        <v>2483.1893985105098</v>
+        <v>2472.1015903856901</v>
       </c>
       <c r="T50" s="2">
-        <v>2647.5484227194302</v>
+        <v>2747.0072120279801</v>
       </c>
     </row>
     <row r="51" spans="2:20" x14ac:dyDescent="0.55000000000000004">
@@ -3063,7 +3071,7 @@
         <v>0</v>
       </c>
       <c r="E51" s="2">
-        <v>1919.6650605561599</v>
+        <v>2051.9689121493898</v>
       </c>
       <c r="G51">
         <v>1</v>
@@ -3075,7 +3083,7 @@
         <v>0</v>
       </c>
       <c r="J51" s="2">
-        <v>2103.6388671044101</v>
+        <v>2284.4054353972001</v>
       </c>
       <c r="L51">
         <v>1</v>
@@ -3087,7 +3095,7 @@
         <v>0</v>
       </c>
       <c r="O51" s="2">
-        <v>1779.3854518575199</v>
+        <v>2265.5057535810101</v>
       </c>
       <c r="Q51">
         <v>1</v>
@@ -3099,7 +3107,7 @@
         <v>0</v>
       </c>
       <c r="T51" s="2">
-        <v>1931.0437097664301</v>
+        <v>2351.33836415717</v>
       </c>
     </row>
     <row r="52" spans="2:20" x14ac:dyDescent="0.55000000000000004">
@@ -3113,7 +3121,7 @@
         <v>0</v>
       </c>
       <c r="E52" s="2">
-        <v>2154.8570833788299</v>
+        <v>2051.9689121493898</v>
       </c>
       <c r="G52">
         <v>0.5</v>
@@ -3125,7 +3133,7 @@
         <v>0</v>
       </c>
       <c r="J52" s="2">
-        <v>1636.3681244136801</v>
+        <v>2284.4054353972001</v>
       </c>
       <c r="L52">
         <v>0.5</v>
@@ -3134,10 +3142,10 @@
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="N52" s="2">
-        <v>193.247074314494</v>
+        <v>699.014088783175</v>
       </c>
       <c r="O52" s="2">
-        <v>1923.20873162308</v>
+        <v>2265.5057535810101</v>
       </c>
       <c r="Q52">
         <v>0.5</v>
@@ -3149,7 +3157,7 @@
         <v>0</v>
       </c>
       <c r="T52" s="2">
-        <v>1999.44433413661</v>
+        <v>2351.33836415717</v>
       </c>
     </row>
     <row r="53" spans="2:20" x14ac:dyDescent="0.55000000000000004">
@@ -3160,10 +3168,10 @@
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="D53" s="2">
-        <v>1858.14801809248</v>
+        <v>0</v>
       </c>
       <c r="E53" s="2">
-        <v>1940.6269772968101</v>
+        <v>2051.9689121493898</v>
       </c>
       <c r="G53">
         <v>0.2</v>
@@ -3172,10 +3180,10 @@
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="I53" s="2">
-        <v>0</v>
+        <v>1891.1401999815</v>
       </c>
       <c r="J53" s="2">
-        <v>1919.2558184409299</v>
+        <v>2284.4054353972001</v>
       </c>
       <c r="L53">
         <v>0.2</v>
@@ -3184,10 +3192,10 @@
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="N53" s="2">
-        <v>2075.1117831450601</v>
+        <v>1893.5855993832899</v>
       </c>
       <c r="O53" s="2">
-        <v>2261.1911964272399</v>
+        <v>2284.4054353972001</v>
       </c>
       <c r="Q53">
         <v>0.2</v>
@@ -3196,10 +3204,10 @@
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="S53" s="2">
-        <v>386.10253911731502</v>
+        <v>792.71994357406697</v>
       </c>
       <c r="T53" s="2">
-        <v>2062.4476842225899</v>
+        <v>2351.33836415717</v>
       </c>
     </row>
     <row r="54" spans="2:20" x14ac:dyDescent="0.55000000000000004">
@@ -3210,10 +3218,10 @@
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="D54" s="2">
-        <v>1865.96096360039</v>
+        <v>923.13094567902203</v>
       </c>
       <c r="E54" s="2">
-        <v>1944.3729683173101</v>
+        <v>2051.9689121493898</v>
       </c>
       <c r="G54">
         <v>0.1</v>
@@ -3222,10 +3230,10 @@
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="I54" s="2">
-        <v>980.20789151881797</v>
+        <v>1949.5355928832701</v>
       </c>
       <c r="J54" s="2">
-        <v>2259.4876987138</v>
+        <v>2284.7340523345802</v>
       </c>
       <c r="L54">
         <v>0.1</v>
@@ -3234,10 +3242,10 @@
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="N54" s="2">
-        <v>2058.7618657328198</v>
+        <v>1949.5355928832701</v>
       </c>
       <c r="O54" s="2">
-        <v>2092.7749601268101</v>
+        <v>2284.7340523345702</v>
       </c>
       <c r="Q54">
         <v>0.1</v>
@@ -3246,10 +3254,10 @@
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="S54" s="2">
-        <v>1652.62444642116</v>
+        <v>1460.6488161187101</v>
       </c>
       <c r="T54" s="2">
-        <v>2502.3297345730598</v>
+        <v>2351.66698109454</v>
       </c>
     </row>
     <row r="55" spans="2:20" x14ac:dyDescent="0.55000000000000004">
@@ -3260,10 +3268,10 @@
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="D55" s="2">
-        <v>2590.3156840153601</v>
+        <v>1474.1642262949699</v>
       </c>
       <c r="E55" s="2">
-        <v>2590.3156840153601</v>
+        <v>2052.2975290867598</v>
       </c>
       <c r="G55">
         <v>0.05</v>
@@ -3272,10 +3280,10 @@
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="I55" s="2">
-        <v>1563.0684592766399</v>
+        <v>2352.0263018611199</v>
       </c>
       <c r="J55" s="2">
-        <v>2027.25916367332</v>
+        <v>2626.9319235034</v>
       </c>
       <c r="L55">
         <v>0.05</v>
@@ -3284,10 +3292,10 @@
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="N55" s="2">
-        <v>2396.52982992754</v>
+        <v>2352.0263018611199</v>
       </c>
       <c r="O55" s="2">
-        <v>2396.52982992754</v>
+        <v>2626.9319235034</v>
       </c>
       <c r="Q55">
         <v>0.05</v>
@@ -3296,10 +3304,10 @@
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="S55" s="2">
-        <v>2412.2872344674201</v>
+        <v>2352.0263018611199</v>
       </c>
       <c r="T55" s="2">
-        <v>2458.1400459266301</v>
+        <v>2626.9319235034</v>
       </c>
     </row>
     <row r="56" spans="2:20" x14ac:dyDescent="0.55000000000000004">
@@ -3310,10 +3318,10 @@
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="D56" s="2">
-        <v>2411.3138345519201</v>
+        <v>2061.1072920461302</v>
       </c>
       <c r="E56" s="2">
-        <v>2782.1569070106898</v>
+        <v>2103.5763904405899</v>
       </c>
       <c r="G56">
         <v>0.01</v>
@@ -3322,10 +3330,10 @@
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="I56" s="2">
-        <v>2039.3988562585801</v>
+        <v>2472.1015903856901</v>
       </c>
       <c r="J56" s="2">
-        <v>2155.7727808760201</v>
+        <v>2747.0072120279801</v>
       </c>
       <c r="L56">
         <v>0.01</v>
@@ -3334,10 +3342,10 @@
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="N56" s="2">
-        <v>2430.44360883737</v>
+        <v>2472.1015903856901</v>
       </c>
       <c r="O56" s="2">
-        <v>2504.6700761114298</v>
+        <v>2747.0072120279801</v>
       </c>
       <c r="Q56">
         <v>0.01</v>
@@ -3346,10 +3354,10 @@
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="S56" s="2">
-        <v>2548.3585931759699</v>
+        <v>2472.1015903856901</v>
       </c>
       <c r="T56" s="2">
-        <v>2679.0887060207901</v>
+        <v>2747.0072120279801</v>
       </c>
     </row>
     <row r="57" spans="2:20" x14ac:dyDescent="0.55000000000000004">
@@ -3360,10 +3368,10 @@
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="D57" s="2">
-        <v>2531.7439387878999</v>
+        <v>2061.1072920461202</v>
       </c>
       <c r="E57" s="2">
-        <v>2531.7439387878999</v>
+        <v>2103.5763904405899</v>
       </c>
       <c r="G57">
         <v>5.0000000000000001E-3</v>
@@ -3372,10 +3380,10 @@
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="I57" s="2">
-        <v>2154.2660988942498</v>
+        <v>2472.1015903856901</v>
       </c>
       <c r="J57" s="2">
-        <v>2216.8297273716398</v>
+        <v>2747.0072120279801</v>
       </c>
       <c r="L57">
         <v>5.0000000000000001E-3</v>
@@ -3384,10 +3392,10 @@
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="N57" s="2">
-        <v>2505.2443657212398</v>
+        <v>2472.1015903856901</v>
       </c>
       <c r="O57" s="2">
-        <v>2596.6504355652701</v>
+        <v>2747.0072120279801</v>
       </c>
       <c r="Q57">
         <v>5.0000000000000001E-3</v>
@@ -3396,10 +3404,10 @@
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="S57" s="2">
-        <v>2431.3440965683699</v>
+        <v>2472.1015903856901</v>
       </c>
       <c r="T57" s="2">
-        <v>2648.1856473508801</v>
+        <v>2747.0072120279801</v>
       </c>
     </row>
     <row r="58" spans="2:20" x14ac:dyDescent="0.55000000000000004">
@@ -3410,10 +3418,10 @@
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="D58" s="2">
-        <v>2478.90391771961</v>
+        <v>2128.04022080609</v>
       </c>
       <c r="E58" s="2">
-        <v>2503.29881255598</v>
+        <v>2170.5093192005602</v>
       </c>
       <c r="G58">
         <v>1E-3</v>
@@ -3422,10 +3430,10 @@
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="I58" s="2">
-        <v>2389.3819941828701</v>
+        <v>2472.1015903856901</v>
       </c>
       <c r="J58" s="2">
-        <v>2434.9866948551298</v>
+        <v>2747.0072120279801</v>
       </c>
       <c r="L58">
         <v>1E-3</v>
@@ -3434,10 +3442,10 @@
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="N58" s="2">
-        <v>2547.3812837523101</v>
+        <v>2472.1015903856901</v>
       </c>
       <c r="O58" s="2">
-        <v>2604.33680803174</v>
+        <v>2747.0072120279801</v>
       </c>
       <c r="Q58">
         <v>1E-3</v>
@@ -3446,10 +3454,10 @@
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="S58" s="2">
-        <v>2475.3130397745999</v>
+        <v>2472.1015903856901</v>
       </c>
       <c r="T58" s="2">
-        <v>2519.6262793574301</v>
+        <v>2747.0072120279801</v>
       </c>
     </row>
     <row r="59" spans="2:20" x14ac:dyDescent="0.55000000000000004">
@@ -3463,7 +3471,7 @@
         <v>0</v>
       </c>
       <c r="E59" s="2">
-        <v>1893.2400629828801</v>
+        <v>2051.9689121493898</v>
       </c>
       <c r="G59">
         <v>1</v>
@@ -3475,7 +3483,7 @@
         <v>0</v>
       </c>
       <c r="J59" s="2">
-        <v>2289.6438287364199</v>
+        <v>2284.4054353972001</v>
       </c>
       <c r="L59">
         <v>1</v>
@@ -3487,7 +3495,7 @@
         <v>0</v>
       </c>
       <c r="O59" s="2">
-        <v>1981.4425865752401</v>
+        <v>2265.5057535810101</v>
       </c>
       <c r="Q59">
         <v>1</v>
@@ -3499,7 +3507,7 @@
         <v>0</v>
       </c>
       <c r="T59" s="2">
-        <v>1935.18480801896</v>
+        <v>2351.33836415717</v>
       </c>
     </row>
     <row r="60" spans="2:20" x14ac:dyDescent="0.55000000000000004">
@@ -3513,7 +3521,7 @@
         <v>0</v>
       </c>
       <c r="E60" s="2">
-        <v>1943.75385869615</v>
+        <v>2051.9689121493898</v>
       </c>
       <c r="G60">
         <v>0.5</v>
@@ -3525,7 +3533,7 @@
         <v>0</v>
       </c>
       <c r="J60" s="2">
-        <v>2085.2019418045502</v>
+        <v>2284.4054353972001</v>
       </c>
       <c r="L60">
         <v>0.5</v>
@@ -3534,10 +3542,10 @@
         <v>1E-3</v>
       </c>
       <c r="N60" s="2">
-        <v>0</v>
+        <v>311.24562421063001</v>
       </c>
       <c r="O60" s="2">
-        <v>2085.29160038283</v>
+        <v>2265.5057535810101</v>
       </c>
       <c r="Q60">
         <v>0.5</v>
@@ -3549,7 +3557,7 @@
         <v>0</v>
       </c>
       <c r="T60" s="2">
-        <v>2317.03178434241</v>
+        <v>2351.33836415717</v>
       </c>
     </row>
     <row r="61" spans="2:20" x14ac:dyDescent="0.55000000000000004">
@@ -3560,10 +3568,10 @@
         <v>1E-3</v>
       </c>
       <c r="D61" s="2">
-        <v>1700.7487382289601</v>
+        <v>0</v>
       </c>
       <c r="E61" s="2">
-        <v>1715.0024686074801</v>
+        <v>2051.9689121493898</v>
       </c>
       <c r="G61">
         <v>0.2</v>
@@ -3572,10 +3580,10 @@
         <v>1E-3</v>
       </c>
       <c r="I61" s="2">
-        <v>0</v>
+        <v>1891.1401999815</v>
       </c>
       <c r="J61" s="2">
-        <v>1892.79982728337</v>
+        <v>2284.4054353972001</v>
       </c>
       <c r="L61">
         <v>0.2</v>
@@ -3584,10 +3592,10 @@
         <v>1E-3</v>
       </c>
       <c r="N61" s="2">
-        <v>1818.3841209505399</v>
+        <v>1893.5855993832899</v>
       </c>
       <c r="O61" s="2">
-        <v>2073.28037394577</v>
+        <v>2284.4054353972001</v>
       </c>
       <c r="Q61">
         <v>0.2</v>
@@ -3596,10 +3604,10 @@
         <v>1E-3</v>
       </c>
       <c r="S61" s="2">
-        <v>567.37918053255999</v>
+        <v>792.71994357406697</v>
       </c>
       <c r="T61" s="2">
-        <v>2417.1459542419202</v>
+        <v>2351.33836415717</v>
       </c>
     </row>
     <row r="62" spans="2:20" x14ac:dyDescent="0.55000000000000004">
@@ -3610,10 +3618,10 @@
         <v>1E-3</v>
       </c>
       <c r="D62" s="2">
-        <v>1827.7099778409399</v>
+        <v>923.13094567902203</v>
       </c>
       <c r="E62" s="2">
-        <v>1864.3924110160301</v>
+        <v>2051.9689121493898</v>
       </c>
       <c r="G62">
         <v>0.1</v>
@@ -3622,10 +3630,10 @@
         <v>1E-3</v>
       </c>
       <c r="I62" s="2">
-        <v>1228.84952347428</v>
+        <v>2016.4685216432299</v>
       </c>
       <c r="J62" s="2">
-        <v>2029.51531386027</v>
+        <v>2351.66698109454</v>
       </c>
       <c r="L62">
         <v>0.1</v>
@@ -3634,10 +3642,10 @@
         <v>1E-3</v>
       </c>
       <c r="N62" s="2">
-        <v>1868.70750603696</v>
+        <v>2016.4685216432299</v>
       </c>
       <c r="O62" s="2">
-        <v>1905.5992067888999</v>
+        <v>2351.66698109454</v>
       </c>
       <c r="Q62">
         <v>0.1</v>
@@ -3646,10 +3654,10 @@
         <v>1E-3</v>
       </c>
       <c r="S62" s="2">
-        <v>2103.0465344622999</v>
+        <v>1460.6488161187101</v>
       </c>
       <c r="T62" s="2">
-        <v>2495.5717504409599</v>
+        <v>2351.66698109454</v>
       </c>
     </row>
     <row r="63" spans="2:20" x14ac:dyDescent="0.55000000000000004">
@@ -3660,10 +3668,10 @@
         <v>1E-3</v>
       </c>
       <c r="D63" s="2">
-        <v>2412.3587307364401</v>
+        <v>1474.1642262949699</v>
       </c>
       <c r="E63" s="2">
-        <v>2485.38192009457</v>
+        <v>2052.2975290867598</v>
       </c>
       <c r="G63">
         <v>0.05</v>
@@ -3672,10 +3680,10 @@
         <v>1E-3</v>
       </c>
       <c r="I63" s="2">
-        <v>1471.43748901461</v>
+        <v>2352.0263018611199</v>
       </c>
       <c r="J63" s="2">
-        <v>2273.9126222974101</v>
+        <v>2626.9319235034</v>
       </c>
       <c r="L63">
         <v>0.05</v>
@@ -3684,10 +3692,10 @@
         <v>1E-3</v>
       </c>
       <c r="N63" s="2">
-        <v>2434.9047380579</v>
+        <v>2352.0263018611199</v>
       </c>
       <c r="O63" s="2">
-        <v>2529.9313504681199</v>
+        <v>2626.9319235034</v>
       </c>
       <c r="Q63">
         <v>0.05</v>
@@ -3696,10 +3704,10 @@
         <v>1E-3</v>
       </c>
       <c r="S63" s="2">
-        <v>2514.7593442370899</v>
+        <v>2352.0263018611199</v>
       </c>
       <c r="T63" s="2">
-        <v>2514.7593442370799</v>
+        <v>2626.9319235034</v>
       </c>
     </row>
     <row r="64" spans="2:20" x14ac:dyDescent="0.55000000000000004">
@@ -3710,10 +3718,10 @@
         <v>1E-3</v>
       </c>
       <c r="D64" s="2">
-        <v>2622.82846303211</v>
+        <v>2061.1072920461302</v>
       </c>
       <c r="E64" s="2">
-        <v>2751.9941571978202</v>
+        <v>2103.5763904405899</v>
       </c>
       <c r="G64">
         <v>0.01</v>
@@ -3722,10 +3730,10 @@
         <v>1E-3</v>
       </c>
       <c r="I64" s="2">
-        <v>2105.97684259168</v>
+        <v>2472.1015903856901</v>
       </c>
       <c r="J64" s="2">
-        <v>2265.2017225128898</v>
+        <v>2747.0072120279801</v>
       </c>
       <c r="L64">
         <v>0.01</v>
@@ -3734,10 +3742,10 @@
         <v>1E-3</v>
       </c>
       <c r="N64" s="2">
-        <v>2494.5515318275602</v>
+        <v>2472.1015903856901</v>
       </c>
       <c r="O64" s="2">
-        <v>2753.0349257090302</v>
+        <v>2747.0072120279801</v>
       </c>
       <c r="Q64">
         <v>0.01</v>
@@ -3746,10 +3754,10 @@
         <v>1E-3</v>
       </c>
       <c r="S64" s="2">
-        <v>2511.2253200526402</v>
+        <v>2472.1015903856901</v>
       </c>
       <c r="T64" s="2">
-        <v>2511.2253200526402</v>
+        <v>2747.0072120279801</v>
       </c>
     </row>
     <row r="65" spans="2:20" x14ac:dyDescent="0.55000000000000004">
@@ -3760,10 +3768,10 @@
         <v>1E-3</v>
       </c>
       <c r="D65" s="2">
-        <v>2483.4029508369599</v>
+        <v>2128.04022080609</v>
       </c>
       <c r="E65" s="2">
-        <v>2568.1474107124</v>
+        <v>2170.5093192005602</v>
       </c>
       <c r="G65">
         <v>5.0000000000000001E-3</v>
@@ -3772,10 +3780,10 @@
         <v>1E-3</v>
       </c>
       <c r="I65" s="2">
-        <v>2358.6798560239899</v>
+        <v>2472.1015903856901</v>
       </c>
       <c r="J65" s="2">
-        <v>2582.7527752598799</v>
+        <v>2747.0072120279801</v>
       </c>
       <c r="L65">
         <v>5.0000000000000001E-3</v>
@@ -3784,10 +3792,10 @@
         <v>1E-3</v>
       </c>
       <c r="N65" s="2">
-        <v>2569.41926856586</v>
+        <v>2472.1015903856901</v>
       </c>
       <c r="O65" s="2">
-        <v>2589.9086803400301</v>
+        <v>2747.0072120279801</v>
       </c>
       <c r="Q65">
         <v>5.0000000000000001E-3</v>
@@ -3796,10 +3804,10 @@
         <v>1E-3</v>
       </c>
       <c r="S65" s="2">
-        <v>2491.7820616858598</v>
+        <v>2472.1015903856901</v>
       </c>
       <c r="T65" s="2">
-        <v>2491.7820616858598</v>
+        <v>2747.0072120279801</v>
       </c>
     </row>
     <row r="66" spans="2:20" x14ac:dyDescent="0.55000000000000004">
@@ -3810,10 +3818,10 @@
         <v>1E-3</v>
       </c>
       <c r="D66" s="2">
-        <v>2541.49455242766</v>
+        <v>2214.1439619288799</v>
       </c>
       <c r="E66" s="2">
-        <v>2627.7001780129699</v>
+        <v>2256.6130603233401</v>
       </c>
       <c r="G66">
         <v>1E-3</v>
@@ -3822,10 +3830,10 @@
         <v>1E-3</v>
       </c>
       <c r="I66" s="2">
-        <v>1841.11050181922</v>
+        <v>2472.1015903856901</v>
       </c>
       <c r="J66" s="2">
-        <v>2059.1903159256199</v>
+        <v>2747.0072120279801</v>
       </c>
       <c r="L66">
         <v>1E-3</v>
@@ -3834,10 +3842,10 @@
         <v>1E-3</v>
       </c>
       <c r="N66" s="2">
-        <v>2493.49902497417</v>
+        <v>2472.1015903856901</v>
       </c>
       <c r="O66" s="2">
-        <v>2830.7592225796998</v>
+        <v>2747.0072120279801</v>
       </c>
       <c r="Q66">
         <v>1E-3</v>
@@ -3846,10 +3854,10 @@
         <v>1E-3</v>
       </c>
       <c r="S66" s="2">
-        <v>2410.6559538524298</v>
+        <v>2472.1015903856901</v>
       </c>
       <c r="T66" s="2">
-        <v>2424.44512385396</v>
+        <v>2747.0072120279801</v>
       </c>
     </row>
   </sheetData>
@@ -3859,8 +3867,8 @@
     </sortState>
   </autoFilter>
   <mergeCells count="4">
+    <mergeCell ref="G1:J1"/>
     <mergeCell ref="B1:E1"/>
-    <mergeCell ref="G1:J1"/>
     <mergeCell ref="L1:O1"/>
     <mergeCell ref="Q1:T1"/>
   </mergeCells>

</xml_diff>